<commit_message>
puntos tumor, mesa aux, cranio en cabeza con rotacion
</commit_message>
<xml_diff>
--- a/puntos del tumor.xlsx
+++ b/puntos del tumor.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\pax\perfils\1198851.CR\Downloads\Short project Brain tumor surgery\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Dropbox\UPC\FIB\Robotica (ROB)\Short project Brain tumor surgery\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -100,13 +100,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -118,7 +115,19 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="5">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -136,12 +145,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B5:D29" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="B5:D29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B5:D157" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="B5:D157"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Diapositiva"/>
-    <tableColumn id="2" name="X"/>
-    <tableColumn id="3" name="Y"/>
+    <tableColumn id="1" name="Diapositiva" dataDxfId="4"/>
+    <tableColumn id="2" name="X" dataDxfId="3"/>
+    <tableColumn id="3" name="Y" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -410,22 +419,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:G28"/>
+  <dimension ref="B4:G156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="2" max="2" width="13" style="1" customWidth="1"/>
+    <col min="3" max="4" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="4"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -437,195 +447,1301 @@
       <c r="D5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
-        <v>89</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="1">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1">
         <v>131.53</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>137.27000000000001</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <v>140</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>136.41999999999999</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>98.11</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>130.44999999999999</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>91.31</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>125.83</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>97.29</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="2">
-        <v>88</v>
-      </c>
-      <c r="C10" s="2">
+      <c r="B10" s="1">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1">
         <v>132.08000000000001</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>105.99</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>136.97</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>102.18</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>135.34</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>94.85</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>129.09</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>90.5</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>124.27</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>95.39</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="2">
-        <v>87</v>
-      </c>
-      <c r="C15" s="2">
+      <c r="B15" s="1">
+        <v>26</v>
+      </c>
+      <c r="C15" s="1">
         <v>129.41</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>101.37</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>137.24</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>94.03</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>128.54</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
         <v>89.14</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>123.65</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>95.2</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <v>122.29</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="1">
         <v>103</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="C20" s="1">
+        <v>130.16999999999999</v>
+      </c>
+      <c r="D20" s="1">
+        <v>88.87</v>
+      </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="C21" s="1">
+        <v>132.08000000000001</v>
+      </c>
+      <c r="D21" s="1">
+        <v>106.8</v>
+      </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="C22" s="1">
+        <v>122.84</v>
+      </c>
+      <c r="D22" s="1">
+        <v>98.38</v>
+      </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="C23" s="1">
+        <v>139.41</v>
+      </c>
+      <c r="D23" s="1">
+        <v>98.92</v>
+      </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="C24" s="1">
+        <v>131.26</v>
+      </c>
+      <c r="D24" s="1">
+        <v>88.59</v>
+      </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="B25" s="1">
+        <v>27</v>
+      </c>
+      <c r="C25" s="1">
+        <v>131.26</v>
+      </c>
+      <c r="D25" s="1">
+        <v>88.32</v>
+      </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+      <c r="C26" s="1">
+        <v>132.35</v>
+      </c>
+      <c r="D26" s="1">
+        <v>108.98</v>
+      </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="C27" s="1">
+        <v>141.59</v>
+      </c>
+      <c r="D27" s="1">
+        <v>98.11</v>
+      </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
+      <c r="C28" s="1">
+        <v>121.21</v>
+      </c>
+      <c r="D28" s="1">
+        <v>98.11</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
+        <v>28</v>
+      </c>
+      <c r="C29" s="1">
+        <v>130.16999999999999</v>
+      </c>
+      <c r="D29" s="1">
+        <v>87.24</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C30" s="1">
+        <v>130.44999999999999</v>
+      </c>
+      <c r="D30" s="1">
+        <v>110.06</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C31" s="1">
+        <v>139.13999999999999</v>
+      </c>
+      <c r="D31" s="1">
+        <v>108.7</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C32" s="1">
+        <v>135.34</v>
+      </c>
+      <c r="D32" s="1">
+        <v>114.14</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="1">
+        <v>143.76</v>
+      </c>
+      <c r="D33" s="1">
+        <v>99.19</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C34" s="1">
+        <v>121.21</v>
+      </c>
+      <c r="D34" s="1">
+        <v>97.83</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="1">
+        <v>29</v>
+      </c>
+      <c r="C35" s="1">
+        <v>129.09</v>
+      </c>
+      <c r="D35" s="1">
+        <v>85.06</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C36" s="1">
+        <v>144.03</v>
+      </c>
+      <c r="D36" s="1">
+        <v>98.75</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C37" s="1">
+        <v>121.21</v>
+      </c>
+      <c r="D37" s="1">
+        <v>98.11</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C38" s="1">
+        <v>129.9</v>
+      </c>
+      <c r="D38" s="1">
+        <v>111.15</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C39" s="1">
+        <v>138.87</v>
+      </c>
+      <c r="D39" s="1">
+        <v>109.79</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C40" s="1">
+        <v>135.34</v>
+      </c>
+      <c r="D40" s="1">
+        <v>114.68</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="1">
+        <v>30</v>
+      </c>
+      <c r="C41" s="1">
+        <v>132.88999999999999</v>
+      </c>
+      <c r="D41" s="1">
+        <v>82.89</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C42" s="1">
+        <v>135.34</v>
+      </c>
+      <c r="D42" s="1">
+        <v>113.87</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C43" s="1">
+        <v>144.31</v>
+      </c>
+      <c r="D43" s="1">
+        <v>99.19</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C44" s="1">
+        <v>120.12</v>
+      </c>
+      <c r="D44" s="1">
+        <v>97.02</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="1">
+        <v>31</v>
+      </c>
+      <c r="C45" s="1">
+        <v>132.35</v>
+      </c>
+      <c r="D45" s="1">
+        <v>81.8</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C46" s="1">
+        <v>134.52000000000001</v>
+      </c>
+      <c r="D46" s="1">
+        <v>114.14</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C47" s="1">
+        <v>145.38999999999999</v>
+      </c>
+      <c r="D47" s="1">
+        <v>98.92</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C48" s="1">
+        <v>120.12</v>
+      </c>
+      <c r="D48" s="1">
+        <v>98.11</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="1">
+        <v>32</v>
+      </c>
+      <c r="C49" s="1">
+        <v>133.97999999999999</v>
+      </c>
+      <c r="D49" s="1">
+        <v>81.260000000000005</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C50" s="1">
+        <v>133.16</v>
+      </c>
+      <c r="D50" s="1">
+        <v>113.6</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C51" s="1">
+        <v>145.66</v>
+      </c>
+      <c r="D51" s="1">
+        <v>97.02</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C52" s="1">
+        <v>118.49</v>
+      </c>
+      <c r="D52" s="1">
+        <v>95.93</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="1">
+        <v>33</v>
+      </c>
+      <c r="C53" s="1">
+        <v>134.25</v>
+      </c>
+      <c r="D53" s="1">
+        <v>80.709999999999994</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C54" s="1">
+        <v>135.07</v>
+      </c>
+      <c r="D54" s="1">
+        <v>114.96</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C55" s="1">
+        <v>146.75</v>
+      </c>
+      <c r="D55" s="1">
+        <v>96.75</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C56" s="1">
+        <v>120.66</v>
+      </c>
+      <c r="D56" s="1">
+        <v>91.58</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C57" s="1">
+        <v>120.12</v>
+      </c>
+      <c r="D57" s="1">
+        <v>104.9</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C58" s="1">
+        <v>113.87</v>
+      </c>
+      <c r="D58" s="1">
+        <v>97.83</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="1">
+        <v>34</v>
+      </c>
+      <c r="C59" s="1">
+        <v>134.79</v>
+      </c>
+      <c r="D59" s="1">
+        <v>79.900000000000006</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C60" s="1">
+        <v>133.97999999999999</v>
+      </c>
+      <c r="D60" s="1">
+        <v>115.23</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C61" s="1">
+        <v>145.66</v>
+      </c>
+      <c r="D61" s="1">
+        <v>103.54</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C62" s="1">
+        <v>143.49</v>
+      </c>
+      <c r="D62" s="1">
+        <v>88.87</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C63" s="1">
+        <v>120.12</v>
+      </c>
+      <c r="D63" s="1">
+        <v>91.86</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C64" s="1">
+        <v>118.49</v>
+      </c>
+      <c r="D64" s="1">
+        <v>104.36</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C65" s="1">
+        <v>112.51</v>
+      </c>
+      <c r="D65" s="1">
+        <v>96.2</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="1">
+        <v>35</v>
+      </c>
+      <c r="C66" s="1">
+        <v>130.44999999999999</v>
+      </c>
+      <c r="D66" s="1">
+        <v>80.709999999999994</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C67" s="1">
+        <v>140.77000000000001</v>
+      </c>
+      <c r="D67" s="1">
+        <v>81.8</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C68" s="1">
+        <v>147.84</v>
+      </c>
+      <c r="D68" s="1">
+        <v>96.75</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C69" s="1">
+        <v>139.96</v>
+      </c>
+      <c r="D69" s="1">
+        <v>110.88</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C70" s="1">
+        <v>126.37</v>
+      </c>
+      <c r="D70" s="1">
+        <v>113.32</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C71" s="1">
+        <v>117.94</v>
+      </c>
+      <c r="D71" s="1">
+        <v>103.81</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C72" s="1">
+        <v>111.97</v>
+      </c>
+      <c r="D72" s="1">
+        <v>99.19</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C73" s="1">
+        <v>119.3</v>
+      </c>
+      <c r="D73" s="1">
+        <v>91.04</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="1">
+        <v>36</v>
+      </c>
+      <c r="C74" s="1">
+        <v>133.71</v>
+      </c>
+      <c r="D74" s="1">
+        <v>80.17</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C75" s="1">
+        <v>147.84</v>
+      </c>
+      <c r="D75" s="1">
+        <v>95.66</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C76" s="1">
+        <v>139.69</v>
+      </c>
+      <c r="D76" s="1">
+        <v>113.87</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C77" s="1">
+        <v>125.09</v>
+      </c>
+      <c r="D77" s="1">
+        <v>112.7</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C78" s="1">
+        <v>119.85</v>
+      </c>
+      <c r="D78" s="1">
+        <v>104.9</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C79" s="1">
+        <v>111.97</v>
+      </c>
+      <c r="D79" s="1">
+        <v>99.74</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C80" s="1">
+        <v>119.03</v>
+      </c>
+      <c r="D80" s="1">
+        <v>91.87</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="1">
+        <v>37</v>
+      </c>
+      <c r="C81" s="1">
+        <v>133.71</v>
+      </c>
+      <c r="D81" s="1">
+        <v>80.44</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C82" s="1">
+        <v>148.38</v>
+      </c>
+      <c r="D82" s="1">
+        <v>97.56</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C83" s="1">
+        <v>142.13</v>
+      </c>
+      <c r="D83" s="1">
+        <v>109.79</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C84" s="1">
+        <v>125.55</v>
+      </c>
+      <c r="D84" s="1">
+        <v>114.14</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C85" s="1">
+        <v>118.49</v>
+      </c>
+      <c r="D85" s="1">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C86" s="1">
+        <v>113.6</v>
+      </c>
+      <c r="D86" s="1">
+        <v>99.46</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C87" s="1">
+        <v>118.76</v>
+      </c>
+      <c r="D87" s="1">
+        <v>92.4</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B88" s="1">
+        <v>38</v>
+      </c>
+      <c r="C88" s="1">
+        <v>128.82</v>
+      </c>
+      <c r="D88" s="1">
+        <v>80.989999999999995</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C89" s="1">
+        <v>138.6</v>
+      </c>
+      <c r="D89" s="1">
+        <v>81.8</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C90" s="1">
+        <v>148.65</v>
+      </c>
+      <c r="D90" s="1">
+        <v>98.11</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C91" s="1">
+        <v>140.22999999999999</v>
+      </c>
+      <c r="D91" s="1">
+        <v>113.6</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C92" s="1">
+        <v>126.37</v>
+      </c>
+      <c r="D92" s="1">
+        <v>114.96</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C93" s="1">
+        <v>118.76</v>
+      </c>
+      <c r="D93" s="1">
+        <v>102.45</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C94" s="1">
+        <v>114.68</v>
+      </c>
+      <c r="D94" s="1">
+        <v>97.29</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C95" s="1">
+        <v>118.22</v>
+      </c>
+      <c r="D95" s="1">
+        <v>93.21</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C96" s="1">
+        <v>123.38</v>
+      </c>
+      <c r="D96" s="1">
+        <v>82.62</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B97" s="1">
+        <v>39</v>
+      </c>
+      <c r="C97" s="1">
+        <v>123.38</v>
+      </c>
+      <c r="D97" s="1">
+        <v>82.62</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C98" s="1">
+        <v>132.88999999999999</v>
+      </c>
+      <c r="D98" s="1">
+        <v>80.989999999999995</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C99" s="1">
+        <v>142.68</v>
+      </c>
+      <c r="D99" s="1">
+        <v>88.59</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C100" s="1">
+        <v>148.93</v>
+      </c>
+      <c r="D100" s="1">
+        <v>99.46</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C101" s="1">
+        <v>140.22999999999999</v>
+      </c>
+      <c r="D101" s="1">
+        <v>113.6</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C102" s="1">
+        <v>125.01</v>
+      </c>
+      <c r="D102" s="1">
+        <v>114.14</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C103" s="1">
+        <v>116.86</v>
+      </c>
+      <c r="D103" s="1">
+        <v>98.11</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B104" s="1">
+        <v>40</v>
+      </c>
+      <c r="C104" s="1">
+        <v>125.83</v>
+      </c>
+      <c r="D104" s="1">
+        <v>81.53</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C105" s="1">
+        <v>139.41</v>
+      </c>
+      <c r="D105" s="1">
+        <v>83.7</v>
+      </c>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C106" s="1">
+        <v>146.47999999999999</v>
+      </c>
+      <c r="D106" s="1">
+        <v>92.13</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C107" s="1">
+        <v>145.38999999999999</v>
+      </c>
+      <c r="D107" s="1">
+        <v>105.72</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C108" s="1">
+        <v>139.96</v>
+      </c>
+      <c r="D108" s="1">
+        <v>113.6</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C109" s="1">
+        <v>124.74</v>
+      </c>
+      <c r="D109" s="1">
+        <v>112.51</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C110" s="1">
+        <v>117.94</v>
+      </c>
+      <c r="D110" s="1">
+        <v>102.18</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C111" s="1">
+        <v>118.49</v>
+      </c>
+      <c r="D111" s="1">
+        <v>88.32</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B112" s="1">
+        <v>41</v>
+      </c>
+      <c r="C112" s="1">
+        <v>125.28</v>
+      </c>
+      <c r="D112" s="1">
+        <v>82.34</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C113" s="1">
+        <v>138.33000000000001</v>
+      </c>
+      <c r="D113" s="1">
+        <v>83.43</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C114" s="1">
+        <v>147.02000000000001</v>
+      </c>
+      <c r="D114" s="1">
+        <v>93.21</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C115" s="1">
+        <v>144.85</v>
+      </c>
+      <c r="D115" s="1">
+        <v>105.72</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C116" s="1">
+        <v>137.51</v>
+      </c>
+      <c r="D116" s="1">
+        <v>113.05</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C117" s="1">
+        <v>126.1</v>
+      </c>
+      <c r="D117" s="1">
+        <v>113.05</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C118" s="1">
+        <v>117.4</v>
+      </c>
+      <c r="D118" s="1">
+        <v>100.28</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C119" s="1">
+        <v>120.12</v>
+      </c>
+      <c r="D119" s="1">
+        <v>87.24</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B120" s="1">
+        <v>42</v>
+      </c>
+      <c r="C120" s="1">
+        <v>125.83</v>
+      </c>
+      <c r="D120" s="1">
+        <v>82.34</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C121" s="1">
+        <v>145.66</v>
+      </c>
+      <c r="D121" s="1">
+        <v>91.58</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C122" s="1">
+        <v>144.31</v>
+      </c>
+      <c r="D122" s="1">
+        <v>105.44</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C123" s="1">
+        <v>129.09</v>
+      </c>
+      <c r="D123" s="1">
+        <v>113.05</v>
+      </c>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C124" s="1">
+        <v>118.22</v>
+      </c>
+      <c r="D124" s="1">
+        <v>100.01</v>
+      </c>
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B125" s="1">
+        <v>43</v>
+      </c>
+      <c r="C125" s="1">
+        <v>128.82</v>
+      </c>
+      <c r="D125" s="1">
+        <v>82.07</v>
+      </c>
+    </row>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C126" s="1">
+        <v>136.97</v>
+      </c>
+      <c r="D126" s="1">
+        <v>85.88</v>
+      </c>
+    </row>
+    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C127" s="1">
+        <v>146.75</v>
+      </c>
+      <c r="D127" s="1">
+        <v>96.75</v>
+      </c>
+    </row>
+    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C128" s="1">
+        <v>140.77000000000001</v>
+      </c>
+      <c r="D128" s="1">
+        <v>107.35</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C129" s="1">
+        <v>129.63</v>
+      </c>
+      <c r="D129" s="1">
+        <v>112.24</v>
+      </c>
+    </row>
+    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C130" s="1">
+        <v>119.3</v>
+      </c>
+      <c r="D130" s="1">
+        <v>98.38</v>
+      </c>
+    </row>
+    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C131" s="1">
+        <v>121.48</v>
+      </c>
+      <c r="D131" s="1">
+        <v>86.96</v>
+      </c>
+    </row>
+    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B132" s="1">
+        <v>44</v>
+      </c>
+      <c r="C132" s="1">
+        <v>130.16999999999999</v>
+      </c>
+      <c r="D132" s="1">
+        <v>82.62</v>
+      </c>
+    </row>
+    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C133" s="1">
+        <v>136.69999999999999</v>
+      </c>
+      <c r="D133" s="1">
+        <v>86.69</v>
+      </c>
+    </row>
+    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C134" s="1">
+        <v>146.47999999999999</v>
+      </c>
+      <c r="D134" s="1">
+        <v>97.83</v>
+      </c>
+    </row>
+    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C135" s="1">
+        <v>133.97999999999999</v>
+      </c>
+      <c r="D135" s="1">
+        <v>110.88</v>
+      </c>
+    </row>
+    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C136" s="1">
+        <v>122.56</v>
+      </c>
+      <c r="D136" s="1">
+        <v>103.81</v>
+      </c>
+    </row>
+    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C137" s="1">
+        <v>119.58</v>
+      </c>
+      <c r="D137" s="1">
+        <v>90.77</v>
+      </c>
+    </row>
+    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B138" s="1">
+        <v>45</v>
+      </c>
+      <c r="C138" s="1">
+        <v>128.27000000000001</v>
+      </c>
+      <c r="D138" s="1">
+        <v>82.62</v>
+      </c>
+    </row>
+    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C139" s="1">
+        <v>135.88</v>
+      </c>
+      <c r="D139" s="1">
+        <v>87.78</v>
+      </c>
+    </row>
+    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C140" s="1">
+        <v>144.85</v>
+      </c>
+      <c r="D140" s="1">
+        <v>95.39</v>
+      </c>
+    </row>
+    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C141" s="1">
+        <v>138.06</v>
+      </c>
+      <c r="D141" s="1">
+        <v>106.06</v>
+      </c>
+    </row>
+    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C142" s="1">
+        <v>125.55</v>
+      </c>
+      <c r="D142" s="1">
+        <v>107.35</v>
+      </c>
+    </row>
+    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C143" s="1">
+        <v>120.66</v>
+      </c>
+      <c r="D143" s="1">
+        <v>92.67</v>
+      </c>
+    </row>
+    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B144" s="1">
+        <v>46</v>
+      </c>
+      <c r="C144" s="1">
+        <v>103.17</v>
+      </c>
+      <c r="D144" s="1">
+        <v>83.16</v>
+      </c>
+    </row>
+    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C145" s="1">
+        <v>137.24</v>
+      </c>
+      <c r="D145" s="1">
+        <v>90.77</v>
+      </c>
+    </row>
+    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C146" s="1">
+        <v>142.94999999999999</v>
+      </c>
+      <c r="D146" s="1">
+        <v>96.2</v>
+      </c>
+    </row>
+    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C147" s="1">
+        <v>130.99</v>
+      </c>
+      <c r="D147" s="1">
+        <v>107.62</v>
+      </c>
+    </row>
+    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C148" s="1">
+        <v>120.93</v>
+      </c>
+      <c r="D148" s="1">
+        <v>94.85</v>
+      </c>
+    </row>
+    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B149" s="1">
+        <v>47</v>
+      </c>
+      <c r="C149" s="1">
+        <v>130.44999999999999</v>
+      </c>
+      <c r="D149" s="1">
+        <v>84.79</v>
+      </c>
+    </row>
+    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C150" s="1">
+        <v>138.33000000000001</v>
+      </c>
+      <c r="D150" s="1">
+        <v>95.93</v>
+      </c>
+    </row>
+    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C151" s="1">
+        <v>131.26</v>
+      </c>
+      <c r="D151" s="1">
+        <v>103.54</v>
+      </c>
+    </row>
+    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C152" s="1">
+        <v>123.38</v>
+      </c>
+      <c r="D152" s="1">
+        <v>94.03</v>
+      </c>
+    </row>
+    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B153" s="1">
+        <v>48</v>
+      </c>
+      <c r="C153" s="1">
+        <v>130.16999999999999</v>
+      </c>
+      <c r="D153" s="1">
+        <v>85.88</v>
+      </c>
+    </row>
+    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C154" s="1">
+        <v>136.15</v>
+      </c>
+      <c r="D154" s="1">
+        <v>94.57</v>
+      </c>
+    </row>
+    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C155" s="1">
+        <v>127.46</v>
+      </c>
+      <c r="D155" s="1">
+        <v>101.64</v>
+      </c>
+    </row>
+    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C156" s="1">
+        <v>123.92</v>
+      </c>
+      <c r="D156" s="1">
+        <v>92.13</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
añadiendo fiducial al excel
</commit_message>
<xml_diff>
--- a/puntos del tumor.xlsx
+++ b/puntos del tumor.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Diapositiva</t>
   </si>
@@ -45,6 +45,15 @@
   </si>
   <si>
     <t>Escala</t>
+  </si>
+  <si>
+    <t>fiducial</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -145,12 +154,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B5:D157" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B5:D157" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="B5:D157"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Diapositiva" dataDxfId="4"/>
-    <tableColumn id="2" name="X" dataDxfId="3"/>
-    <tableColumn id="3" name="Y" dataDxfId="2"/>
+    <tableColumn id="1" name="Diapositiva" dataDxfId="2"/>
+    <tableColumn id="2" name="X" dataDxfId="1"/>
+    <tableColumn id="3" name="Y" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -419,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:G156"/>
+  <dimension ref="B4:H156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,13 +440,13 @@
     <col min="3" max="4" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="F4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -454,7 +463,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>24</v>
       </c>
@@ -471,7 +480,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C7" s="1">
         <v>136.41999999999999</v>
       </c>
@@ -479,7 +488,7 @@
         <v>98.11</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C8" s="1">
         <v>130.44999999999999</v>
       </c>
@@ -487,7 +496,7 @@
         <v>91.31</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
         <v>125.83</v>
       </c>
@@ -495,7 +504,7 @@
         <v>97.29</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>25</v>
       </c>
@@ -505,16 +514,31 @@
       <c r="D10" s="1">
         <v>105.99</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="1">
+        <v>121.57</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C11" s="1">
         <v>136.97</v>
       </c>
       <c r="D11" s="1">
         <v>102.18</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="1">
+        <v>208.49</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C12" s="1">
         <v>135.34</v>
       </c>
@@ -522,7 +546,7 @@
         <v>94.85</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C13" s="1">
         <v>129.09</v>
       </c>
@@ -530,7 +554,7 @@
         <v>90.5</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C14" s="1">
         <v>124.27</v>
       </c>
@@ -538,7 +562,7 @@
         <v>95.39</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>26</v>
       </c>
@@ -549,7 +573,7 @@
         <v>101.37</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C16" s="1">
         <v>137.24</v>
       </c>

</xml_diff>

<commit_message>
tumor centrado en el oringe
</commit_message>
<xml_diff>
--- a/puntos del tumor.xlsx
+++ b/puntos del tumor.xlsx
@@ -73,10 +73,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="171" formatCode="0.0000"/>
-    <numFmt numFmtId="172" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,6 +87,14 @@
     <font>
       <b/>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -125,7 +133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -133,19 +141,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -197,7 +208,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B5:G157" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="B5:G157"/>
   <sortState ref="B6:G157">
-    <sortCondition descending="1" ref="G5:G157"/>
+    <sortCondition ref="B5:B157"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" name="Diapositiva" dataDxfId="5"/>
@@ -480,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:N157"/>
+  <dimension ref="B3:N157"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,11 +506,16 @@
     <col min="10" max="10" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>0.109949743</v>
+      </c>
+    </row>
     <row r="4" spans="2:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="3"/>
+      <c r="K4" s="7"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -532,22 +548,22 @@
         <v>24</v>
       </c>
       <c r="C6" s="1">
-        <v>131.53</v>
+        <v>131.09</v>
       </c>
       <c r="D6" s="1">
-        <v>137.27000000000001</v>
-      </c>
-      <c r="E6" s="7">
+        <v>103.13</v>
+      </c>
+      <c r="E6" s="6">
         <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
         <v>3.3599999999999991E-2</v>
       </c>
       <c r="F6" s="1">
         <f>+((C6*$J$6)/$K$6)/1000</f>
-        <v>0.14017339999999998</v>
+        <v>0.1397044857142857</v>
       </c>
       <c r="G6" s="1">
         <f>+((D6*$J$6)/$K$6)/1000</f>
-        <v>0.14629060000000002</v>
+        <v>0.10990711428571427</v>
       </c>
       <c r="J6" s="2">
         <v>149.19999999999999</v>
@@ -558,71 +574,71 @@
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
-        <v>34</v>
-      </c>
-      <c r="C7" s="1">
-        <v>133.97999999999999</v>
+        <v>24</v>
+      </c>
+      <c r="C7" s="8">
+        <v>136.41999999999999</v>
       </c>
       <c r="D7" s="1">
-        <v>115.23</v>
-      </c>
-      <c r="E7" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.7599999999999996E-2</v>
+        <v>98.11</v>
+      </c>
+      <c r="E7" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>3.3599999999999991E-2</v>
       </c>
       <c r="F7" s="1">
         <f>+((C7*$J$6)/$K$6)/1000</f>
-        <v>0.14278439999999998</v>
+        <v>0.14538474285714284</v>
       </c>
       <c r="G7" s="1">
         <f>+((D7*$J$6)/$K$6)/1000</f>
-        <v>0.12280225714285713</v>
+        <v>0.10455722857142857</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1">
-        <v>126.37</v>
+        <v>125.83</v>
       </c>
       <c r="D8" s="1">
-        <v>114.96</v>
-      </c>
-      <c r="E8" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.3199999999999997E-2</v>
+        <v>97.29</v>
+      </c>
+      <c r="E8" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>3.3599999999999991E-2</v>
       </c>
       <c r="F8" s="1">
         <f>+((C8*$J$6)/$K$6)/1000</f>
-        <v>0.13467431428571427</v>
+        <v>0.13409882857142855</v>
       </c>
       <c r="G8" s="1">
         <f>+((D8*$J$6)/$K$6)/1000</f>
-        <v>0.12251451428571429</v>
+        <v>0.10368334285714285</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1">
-        <v>135.07</v>
+        <v>130.44999999999999</v>
       </c>
       <c r="D9" s="1">
-        <v>114.96</v>
-      </c>
-      <c r="E9" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.6199999999999998E-2</v>
+        <v>91.31</v>
+      </c>
+      <c r="E9" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>3.3599999999999991E-2</v>
       </c>
       <c r="F9" s="1">
         <f>+((C9*$J$6)/$K$6)/1000</f>
-        <v>0.14394602857142855</v>
+        <v>0.13902242857142855</v>
       </c>
       <c r="G9" s="1">
         <f>+((D9*$J$6)/$K$6)/1000</f>
-        <v>0.12251451428571429</v>
+        <v>9.7310371428571435E-2</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>2</v>
@@ -636,25 +652,25 @@
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C10" s="1">
-        <v>135.34</v>
+        <v>132.08000000000001</v>
       </c>
       <c r="D10" s="1">
-        <v>114.68</v>
-      </c>
-      <c r="E10" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.0599999999999997E-2</v>
+        <v>105.99</v>
+      </c>
+      <c r="E10" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="F10" s="1">
         <f>+((C10*$J$6)/$K$6)/1000</f>
-        <v>0.14423377142857144</v>
+        <v>0.14075954285714287</v>
       </c>
       <c r="G10" s="1">
         <f>+((D10*$J$6)/$K$6)/1000</f>
-        <v>0.1222161142857143</v>
+        <v>0.11295505714285713</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>8</v>
@@ -665,36 +681,36 @@
       <c r="L10" s="1">
         <v>122.28</v>
       </c>
-      <c r="M10" s="4">
+      <c r="M10" s="3">
         <f>+(L10*$J$6)/$K$6</f>
         <v>130.31554285714284</v>
       </c>
-      <c r="N10" s="5">
+      <c r="N10" s="4">
         <f>+M10/1000</f>
         <v>0.13031554285714284</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1">
-        <v>125.01</v>
+        <v>136.97</v>
       </c>
       <c r="D11" s="1">
-        <v>114.14</v>
-      </c>
-      <c r="E11" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.4599999999999996E-2</v>
+        <v>102.18</v>
+      </c>
+      <c r="E11" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="F11" s="1">
         <f>+((C11*$J$6)/$K$6)/1000</f>
-        <v>0.13322494285714284</v>
+        <v>0.14597088571428571</v>
       </c>
       <c r="G11" s="1">
         <f>+((D11*$J$6)/$K$6)/1000</f>
-        <v>0.12164062857142856</v>
+        <v>0.10889468571428572</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>5</v>
@@ -702,84 +718,84 @@
       <c r="L11" s="1">
         <v>208.09</v>
       </c>
-      <c r="M11" s="4">
+      <c r="M11" s="3">
         <f>+(L11*$J$6)/$K$6</f>
         <v>221.76448571428571</v>
       </c>
-      <c r="N11" s="5">
+      <c r="N11" s="4">
         <f>+M11/1000</f>
         <v>0.22176448571428573</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1">
-        <v>125.55</v>
+        <v>124.27</v>
       </c>
       <c r="D12" s="1">
-        <v>114.14</v>
-      </c>
-      <c r="E12" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.1799999999999999E-2</v>
+        <v>95.39</v>
+      </c>
+      <c r="E12" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="F12" s="1">
         <f>+((C12*$J$6)/$K$6)/1000</f>
-        <v>0.13380042857142857</v>
+        <v>0.13243631428571428</v>
       </c>
       <c r="G12" s="1">
         <f>+((D12*$J$6)/$K$6)/1000</f>
-        <v>0.12164062857142856</v>
+        <v>0.10165848571428571</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1">
-        <v>134.52000000000001</v>
+        <v>135.34</v>
       </c>
       <c r="D13" s="1">
-        <v>114.14</v>
-      </c>
-      <c r="E13" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.3400000000000001E-2</v>
+        <v>94.85</v>
+      </c>
+      <c r="E13" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="F13" s="1">
         <f>+((C13*$J$6)/$K$6)/1000</f>
-        <v>0.14335988571428571</v>
+        <v>0.14423377142857144</v>
       </c>
       <c r="G13" s="1">
         <f>+((D13*$J$6)/$K$6)/1000</f>
-        <v>0.12164062857142856</v>
+        <v>0.10108299999999999</v>
       </c>
     </row>
     <row r="14" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C14" s="1">
-        <v>135.34</v>
+        <v>129.09</v>
       </c>
       <c r="D14" s="1">
-        <v>114.14</v>
-      </c>
-      <c r="E14" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>3.9199999999999999E-2</v>
+        <v>90.5</v>
+      </c>
+      <c r="E14" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="F14" s="1">
         <f>+((C14*$J$6)/$K$6)/1000</f>
-        <v>0.14423377142857144</v>
+        <v>0.13757305714285711</v>
       </c>
       <c r="G14" s="1">
         <f>+((D14*$J$6)/$K$6)/1000</f>
-        <v>0.12164062857142856</v>
-      </c>
-      <c r="J14" s="6" t="s">
+        <v>9.6447142857142856E-2</v>
+      </c>
+      <c r="J14" s="5" t="s">
         <v>7</v>
       </c>
       <c r="N14" s="1">
@@ -788,370 +804,370 @@
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C15" s="1">
-        <v>139.69</v>
+        <v>132.08000000000001</v>
       </c>
       <c r="D15" s="1">
-        <v>113.87</v>
-      </c>
-      <c r="E15" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.04E-2</v>
+        <v>106.8</v>
+      </c>
+      <c r="E15" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>3.6400000000000002E-2</v>
       </c>
       <c r="F15" s="1">
         <f>+((C15*$J$6)/$K$6)/1000</f>
-        <v>0.14886962857142857</v>
+        <v>0.14075954285714287</v>
       </c>
       <c r="G15" s="1">
         <f>+((D15*$J$6)/$K$6)/1000</f>
-        <v>0.12135288571428571</v>
+        <v>0.11381828571428569</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C16" s="1">
-        <v>135.34</v>
+        <v>122.29</v>
       </c>
       <c r="D16" s="1">
-        <v>113.87</v>
-      </c>
-      <c r="E16" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.2000000000000003E-2</v>
+        <v>103</v>
+      </c>
+      <c r="E16" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>3.6400000000000002E-2</v>
       </c>
       <c r="F16" s="1">
         <f>+((C16*$J$6)/$K$6)/1000</f>
-        <v>0.14423377142857144</v>
+        <v>0.13032619999999998</v>
       </c>
       <c r="G16" s="1">
         <f>+((D16*$J$6)/$K$6)/1000</f>
-        <v>0.12135288571428571</v>
+        <v>0.10976857142857142</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C17" s="1">
-        <v>139.96</v>
+        <v>129.41</v>
       </c>
       <c r="D17" s="1">
-        <v>113.6</v>
-      </c>
-      <c r="E17" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.6000000000000001E-2</v>
+        <v>101.37</v>
+      </c>
+      <c r="E17" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>3.6400000000000002E-2</v>
       </c>
       <c r="F17" s="1">
         <f>+((C17*$J$6)/$K$6)/1000</f>
-        <v>0.14915737142857141</v>
+        <v>0.13791408571428571</v>
       </c>
       <c r="G17" s="1">
         <f>+((D17*$J$6)/$K$6)/1000</f>
-        <v>0.12106514285714284</v>
+        <v>0.10803145714285714</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C18" s="1">
-        <v>140.22999999999999</v>
+        <v>139.41</v>
       </c>
       <c r="D18" s="1">
-        <v>113.6</v>
-      </c>
-      <c r="E18" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.4599999999999996E-2</v>
+        <v>98.92</v>
+      </c>
+      <c r="E18" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>3.6400000000000002E-2</v>
       </c>
       <c r="F18" s="1">
         <f>+((C18*$J$6)/$K$6)/1000</f>
-        <v>0.14944511428571425</v>
+        <v>0.14857122857142854</v>
       </c>
       <c r="G18" s="1">
         <f>+((D18*$J$6)/$K$6)/1000</f>
-        <v>0.12106514285714284</v>
+        <v>0.10542045714285715</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C19" s="1">
-        <v>140.22999999999999</v>
+        <v>122.84</v>
       </c>
       <c r="D19" s="1">
-        <v>113.6</v>
-      </c>
-      <c r="E19" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.3199999999999997E-2</v>
+        <v>98.38</v>
+      </c>
+      <c r="E19" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>3.6400000000000002E-2</v>
       </c>
       <c r="F19" s="1">
         <f>+((C19*$J$6)/$K$6)/1000</f>
-        <v>0.14944511428571425</v>
+        <v>0.13091234285714284</v>
       </c>
       <c r="G19" s="1">
         <f>+((D19*$J$6)/$K$6)/1000</f>
-        <v>0.12106514285714284</v>
+        <v>0.10484497142857141</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C20" s="1">
-        <v>133.16</v>
+        <v>123.65</v>
       </c>
       <c r="D20" s="1">
-        <v>113.6</v>
-      </c>
-      <c r="E20" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.48E-2</v>
+        <v>95.2</v>
+      </c>
+      <c r="E20" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>3.6400000000000002E-2</v>
       </c>
       <c r="F20" s="1">
         <f>+((C20*$J$6)/$K$6)/1000</f>
-        <v>0.14191051428571427</v>
+        <v>0.13177557142857144</v>
       </c>
       <c r="G20" s="1">
         <f>+((D20*$J$6)/$K$6)/1000</f>
-        <v>0.12106514285714284</v>
+        <v>0.101456</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C21" s="1">
-        <v>126.37</v>
+        <v>137.24</v>
       </c>
       <c r="D21" s="1">
-        <v>113.32</v>
-      </c>
-      <c r="E21" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.9000000000000002E-2</v>
+        <v>94.03</v>
+      </c>
+      <c r="E21" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>3.6400000000000002E-2</v>
       </c>
       <c r="F21" s="1">
         <f>+((C21*$J$6)/$K$6)/1000</f>
-        <v>0.13467431428571427</v>
+        <v>0.14625862857142857</v>
       </c>
       <c r="G21" s="1">
         <f>+((D21*$J$6)/$K$6)/1000</f>
-        <v>0.12076674285714284</v>
+        <v>0.10020911428571427</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C22" s="1">
-        <v>129.09</v>
+        <v>128.54</v>
       </c>
       <c r="D22" s="1">
-        <v>113.05</v>
-      </c>
-      <c r="E22" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.8799999999999998E-2</v>
+        <v>89.14</v>
+      </c>
+      <c r="E22" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>3.6400000000000002E-2</v>
       </c>
       <c r="F22" s="1">
         <f>+((C22*$J$6)/$K$6)/1000</f>
-        <v>0.13757305714285711</v>
+        <v>0.13698691428571427</v>
       </c>
       <c r="G22" s="1">
         <f>+((D22*$J$6)/$K$6)/1000</f>
-        <v>0.12047899999999999</v>
+        <v>9.4997771428571409E-2</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C23" s="1">
-        <v>137.51</v>
+        <v>130.16999999999999</v>
       </c>
       <c r="D23" s="1">
-        <v>113.05</v>
-      </c>
-      <c r="E23" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.74E-2</v>
+        <v>88.87</v>
+      </c>
+      <c r="E23" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>3.6400000000000002E-2</v>
       </c>
       <c r="F23" s="1">
         <f>+((C23*$J$6)/$K$6)/1000</f>
-        <v>0.14654637142857141</v>
+        <v>0.13872402857142857</v>
       </c>
       <c r="G23" s="1">
         <f>+((D23*$J$6)/$K$6)/1000</f>
-        <v>0.12047899999999999</v>
+        <v>9.4710028571428587E-2</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C24" s="1">
-        <v>126.1</v>
+        <v>131.26</v>
       </c>
       <c r="D24" s="1">
-        <v>113.05</v>
-      </c>
-      <c r="E24" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.74E-2</v>
+        <v>88.59</v>
+      </c>
+      <c r="E24" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>3.6400000000000002E-2</v>
       </c>
       <c r="F24" s="1">
         <f>+((C24*$J$6)/$K$6)/1000</f>
-        <v>0.13438657142857141</v>
+        <v>0.13988565714285714</v>
       </c>
       <c r="G24" s="1">
         <f>+((D24*$J$6)/$K$6)/1000</f>
-        <v>0.12047899999999999</v>
+        <v>9.4411628571428569E-2</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C25" s="1">
-        <v>125.09</v>
+        <v>132.35</v>
       </c>
       <c r="D25" s="1">
-        <v>112.7</v>
-      </c>
-      <c r="E25" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.04E-2</v>
+        <v>108.98</v>
+      </c>
+      <c r="E25" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>3.78E-2</v>
       </c>
       <c r="F25" s="1">
         <f>+((C25*$J$6)/$K$6)/1000</f>
-        <v>0.13331020000000002</v>
+        <v>0.14104728571428571</v>
       </c>
       <c r="G25" s="1">
         <f>+((D25*$J$6)/$K$6)/1000</f>
-        <v>0.12010599999999999</v>
+        <v>0.11614154285714286</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C26" s="1">
-        <v>124.74</v>
+        <v>141.59</v>
       </c>
       <c r="D26" s="1">
-        <v>112.51</v>
-      </c>
-      <c r="E26" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.6000000000000001E-2</v>
+        <v>98.11</v>
+      </c>
+      <c r="E26" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>3.78E-2</v>
       </c>
       <c r="F26" s="1">
         <f>+((C26*$J$6)/$K$6)/1000</f>
-        <v>0.13293719999999998</v>
+        <v>0.15089448571428571</v>
       </c>
       <c r="G26" s="1">
         <f>+((D26*$J$6)/$K$6)/1000</f>
-        <v>0.11990351428571427</v>
+        <v>0.10455722857142857</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C27" s="1">
-        <v>129.63</v>
+        <v>121.21</v>
       </c>
       <c r="D27" s="1">
-        <v>112.24</v>
-      </c>
-      <c r="E27" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.0199999999999997E-2</v>
+        <v>98.11</v>
+      </c>
+      <c r="E27" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>3.78E-2</v>
       </c>
       <c r="F27" s="1">
         <f>+((C27*$J$6)/$K$6)/1000</f>
-        <v>0.13814854285714284</v>
+        <v>0.12917522857142857</v>
       </c>
       <c r="G27" s="1">
         <f>+((D27*$J$6)/$K$6)/1000</f>
-        <v>0.11961577142857142</v>
+        <v>0.10455722857142857</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C28" s="1">
-        <v>129.9</v>
+        <v>131.26</v>
       </c>
       <c r="D28" s="1">
-        <v>111.15</v>
-      </c>
-      <c r="E28" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.0599999999999997E-2</v>
+        <v>88.32</v>
+      </c>
+      <c r="E28" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>3.78E-2</v>
       </c>
       <c r="F28" s="1">
         <f>+((C28*$J$6)/$K$6)/1000</f>
-        <v>0.13843628571428571</v>
+        <v>0.13988565714285714</v>
       </c>
       <c r="G28" s="1">
         <f>+((D28*$J$6)/$K$6)/1000</f>
-        <v>0.11845414285714284</v>
+        <v>9.4123885714285691E-2</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C29" s="1">
-        <v>133.97999999999999</v>
+        <v>135.34</v>
       </c>
       <c r="D29" s="1">
-        <v>110.88</v>
-      </c>
-      <c r="E29" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.1599999999999995E-2</v>
+        <v>114.14</v>
+      </c>
+      <c r="E29" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>3.9199999999999999E-2</v>
       </c>
       <c r="F29" s="1">
         <f>+((C29*$J$6)/$K$6)/1000</f>
-        <v>0.14278439999999998</v>
+        <v>0.14423377142857144</v>
       </c>
       <c r="G29" s="1">
         <f>+((D29*$J$6)/$K$6)/1000</f>
-        <v>0.11816639999999999</v>
+        <v>0.12164062857142856</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C30" s="1">
-        <v>139.96</v>
+        <v>130.44999999999999</v>
       </c>
       <c r="D30" s="1">
-        <v>110.88</v>
-      </c>
-      <c r="E30" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.9000000000000002E-2</v>
+        <v>110.06</v>
+      </c>
+      <c r="E30" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>3.9199999999999999E-2</v>
       </c>
       <c r="F30" s="1">
         <f>+((C30*$J$6)/$K$6)/1000</f>
-        <v>0.14915737142857141</v>
+        <v>0.13902242857142855</v>
       </c>
       <c r="G30" s="1">
         <f>+((D30*$J$6)/$K$6)/1000</f>
-        <v>0.11816639999999999</v>
+        <v>0.11729251428571426</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
@@ -1159,1172 +1175,1172 @@
         <v>28</v>
       </c>
       <c r="C31" s="1">
-        <v>130.44999999999999</v>
+        <v>139.13999999999999</v>
       </c>
       <c r="D31" s="1">
-        <v>110.06</v>
-      </c>
-      <c r="E31" s="7">
+        <v>108.7</v>
+      </c>
+      <c r="E31" s="6">
         <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
         <v>3.9199999999999999E-2</v>
       </c>
       <c r="F31" s="1">
         <f>+((C31*$J$6)/$K$6)/1000</f>
-        <v>0.13902242857142855</v>
+        <v>0.14828348571428568</v>
       </c>
       <c r="G31" s="1">
         <f>+((D31*$J$6)/$K$6)/1000</f>
-        <v>0.11729251428571426</v>
+        <v>0.11584314285714285</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="1">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C32" s="1">
-        <v>142.13</v>
+        <v>143.76</v>
       </c>
       <c r="D32" s="1">
-        <v>109.79</v>
-      </c>
-      <c r="E32" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.1799999999999999E-2</v>
+        <v>99.19</v>
+      </c>
+      <c r="E32" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>3.9199999999999999E-2</v>
       </c>
       <c r="F32" s="1">
         <f>+((C32*$J$6)/$K$6)/1000</f>
-        <v>0.15146997142857144</v>
+        <v>0.15320708571428571</v>
       </c>
       <c r="G32" s="1">
         <f>+((D32*$J$6)/$K$6)/1000</f>
-        <v>0.11700477142857144</v>
+        <v>0.10570819999999999</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C33" s="1">
-        <v>138.87</v>
+        <v>121.21</v>
       </c>
       <c r="D33" s="1">
-        <v>109.79</v>
-      </c>
-      <c r="E33" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.0599999999999997E-2</v>
+        <v>97.83</v>
+      </c>
+      <c r="E33" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>3.9199999999999999E-2</v>
       </c>
       <c r="F33" s="1">
         <f>+((C33*$J$6)/$K$6)/1000</f>
-        <v>0.14799574285714287</v>
+        <v>0.12917522857142857</v>
       </c>
       <c r="G33" s="1">
         <f>+((D33*$J$6)/$K$6)/1000</f>
-        <v>0.11700477142857144</v>
+        <v>0.10425882857142857</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C34" s="1">
-        <v>132.35</v>
+        <v>130.16999999999999</v>
       </c>
       <c r="D34" s="1">
-        <v>108.98</v>
-      </c>
-      <c r="E34" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>3.78E-2</v>
+        <v>87.24</v>
+      </c>
+      <c r="E34" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>3.9199999999999999E-2</v>
       </c>
       <c r="F34" s="1">
         <f>+((C34*$J$6)/$K$6)/1000</f>
-        <v>0.14104728571428571</v>
+        <v>0.13872402857142857</v>
       </c>
       <c r="G34" s="1">
         <f>+((D34*$J$6)/$K$6)/1000</f>
-        <v>0.11614154285714286</v>
+        <v>9.2972914285714275E-2</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C35" s="1">
-        <v>139.13999999999999</v>
+        <v>135.34</v>
       </c>
       <c r="D35" s="1">
-        <v>108.7</v>
-      </c>
-      <c r="E35" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>3.9199999999999999E-2</v>
+        <v>114.68</v>
+      </c>
+      <c r="E35" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.0599999999999997E-2</v>
       </c>
       <c r="F35" s="1">
         <f>+((C35*$J$6)/$K$6)/1000</f>
-        <v>0.14828348571428568</v>
+        <v>0.14423377142857144</v>
       </c>
       <c r="G35" s="1">
         <f>+((D35*$J$6)/$K$6)/1000</f>
-        <v>0.11584314285714285</v>
+        <v>0.1222161142857143</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="1">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="C36" s="1">
-        <v>130.99</v>
+        <v>129.9</v>
       </c>
       <c r="D36" s="1">
-        <v>107.62</v>
-      </c>
-      <c r="E36" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.4399999999999985E-2</v>
+        <v>111.15</v>
+      </c>
+      <c r="E36" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.0599999999999997E-2</v>
       </c>
       <c r="F36" s="1">
         <f>+((C36*$J$6)/$K$6)/1000</f>
-        <v>0.13959791428571428</v>
+        <v>0.13843628571428571</v>
       </c>
       <c r="G36" s="1">
         <f>+((D36*$J$6)/$K$6)/1000</f>
-        <v>0.11469217142857141</v>
+        <v>0.11845414285714284</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="C37" s="1">
-        <v>125.55</v>
+        <v>138.87</v>
       </c>
       <c r="D37" s="1">
-        <v>107.35</v>
-      </c>
-      <c r="E37" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.2999999999999987E-2</v>
+        <v>109.79</v>
+      </c>
+      <c r="E37" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.0599999999999997E-2</v>
       </c>
       <c r="F37" s="1">
         <f>+((C37*$J$6)/$K$6)/1000</f>
-        <v>0.13380042857142857</v>
+        <v>0.14799574285714287</v>
       </c>
       <c r="G37" s="1">
         <f>+((D37*$J$6)/$K$6)/1000</f>
-        <v>0.11440442857142856</v>
+        <v>0.11700477142857144</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="1">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C38" s="1">
-        <v>140.77000000000001</v>
+        <v>144.03</v>
       </c>
       <c r="D38" s="1">
-        <v>107.35</v>
-      </c>
-      <c r="E38" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.0199999999999997E-2</v>
+        <v>98.75</v>
+      </c>
+      <c r="E38" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.0599999999999997E-2</v>
       </c>
       <c r="F38" s="1">
         <f>+((C38*$J$6)/$K$6)/1000</f>
-        <v>0.15002059999999998</v>
+        <v>0.15349482857142857</v>
       </c>
       <c r="G38" s="1">
         <f>+((D38*$J$6)/$K$6)/1000</f>
-        <v>0.11440442857142856</v>
+        <v>0.1052392857142857</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C39" s="1">
-        <v>132.08000000000001</v>
+        <v>121.21</v>
       </c>
       <c r="D39" s="1">
-        <v>106.8</v>
-      </c>
-      <c r="E39" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>3.6400000000000002E-2</v>
+        <v>98.11</v>
+      </c>
+      <c r="E39" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.0599999999999997E-2</v>
       </c>
       <c r="F39" s="1">
         <f>+((C39*$J$6)/$K$6)/1000</f>
-        <v>0.14075954285714287</v>
+        <v>0.12917522857142857</v>
       </c>
       <c r="G39" s="1">
         <f>+((D39*$J$6)/$K$6)/1000</f>
-        <v>0.11381828571428569</v>
+        <v>0.10455722857142857</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="1">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="C40" s="1">
-        <v>138.06</v>
+        <v>129.09</v>
       </c>
       <c r="D40" s="1">
-        <v>106.06</v>
-      </c>
-      <c r="E40" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.2999999999999987E-2</v>
+        <v>85.06</v>
+      </c>
+      <c r="E40" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.0599999999999997E-2</v>
       </c>
       <c r="F40" s="1">
         <f>+((C40*$J$6)/$K$6)/1000</f>
-        <v>0.14713251428571428</v>
+        <v>0.13757305714285711</v>
       </c>
       <c r="G40" s="1">
         <f>+((D40*$J$6)/$K$6)/1000</f>
-        <v>0.11302965714285713</v>
+        <v>9.0649657142857137E-2</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="1">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C41" s="1">
-        <v>132.08000000000001</v>
+        <v>135.34</v>
       </c>
       <c r="D41" s="1">
-        <v>105.99</v>
-      </c>
-      <c r="E41" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>3.5000000000000003E-2</v>
+        <v>113.87</v>
+      </c>
+      <c r="E41" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="F41" s="1">
         <f>+((C41*$J$6)/$K$6)/1000</f>
-        <v>0.14075954285714287</v>
+        <v>0.14423377142857144</v>
       </c>
       <c r="G41" s="1">
         <f>+((D41*$J$6)/$K$6)/1000</f>
-        <v>0.11295505714285713</v>
+        <v>0.12135288571428571</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="1">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C42" s="1">
-        <v>144.85</v>
+        <v>144.31</v>
       </c>
       <c r="D42" s="1">
-        <v>105.72</v>
-      </c>
-      <c r="E42" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.74E-2</v>
+        <v>99.19</v>
+      </c>
+      <c r="E42" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="F42" s="1">
         <f>+((C42*$J$6)/$K$6)/1000</f>
-        <v>0.15436871428571428</v>
+        <v>0.15379322857142855</v>
       </c>
       <c r="G42" s="1">
         <f>+((D42*$J$6)/$K$6)/1000</f>
-        <v>0.11266731428571429</v>
+        <v>0.10570819999999999</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" s="1">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C43" s="1">
-        <v>145.38999999999999</v>
+        <v>120.12</v>
       </c>
       <c r="D43" s="1">
-        <v>105.72</v>
-      </c>
-      <c r="E43" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.6000000000000001E-2</v>
+        <v>97.02</v>
+      </c>
+      <c r="E43" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="F43" s="1">
         <f>+((C43*$J$6)/$K$6)/1000</f>
-        <v>0.15494419999999998</v>
+        <v>0.12801360000000001</v>
       </c>
       <c r="G43" s="1">
         <f>+((D43*$J$6)/$K$6)/1000</f>
-        <v>0.11266731428571429</v>
+        <v>0.10339559999999999</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" s="1">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C44" s="1">
-        <v>144.31</v>
+        <v>132.88999999999999</v>
       </c>
       <c r="D44" s="1">
-        <v>105.44</v>
-      </c>
-      <c r="E44" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.8799999999999998E-2</v>
+        <v>82.89</v>
+      </c>
+      <c r="E44" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="F44" s="1">
         <f>+((C44*$J$6)/$K$6)/1000</f>
-        <v>0.15379322857142855</v>
+        <v>0.14162277142857138</v>
       </c>
       <c r="G44" s="1">
         <f>+((D44*$J$6)/$K$6)/1000</f>
-        <v>0.11236891428571429</v>
+        <v>8.8337057142857139E-2</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="1">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C45" s="1">
-        <v>119.85</v>
+        <v>134.52000000000001</v>
       </c>
       <c r="D45" s="1">
-        <v>104.9</v>
-      </c>
-      <c r="E45" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.04E-2</v>
+        <v>114.14</v>
+      </c>
+      <c r="E45" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.3400000000000001E-2</v>
       </c>
       <c r="F45" s="1">
         <f>+((C45*$J$6)/$K$6)/1000</f>
-        <v>0.12772585714285714</v>
+        <v>0.14335988571428571</v>
       </c>
       <c r="G45" s="1">
         <f>+((D45*$J$6)/$K$6)/1000</f>
-        <v>0.11179342857142857</v>
+        <v>0.12164062857142856</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="1">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C46" s="1">
-        <v>120.12</v>
+        <v>145.38999999999999</v>
       </c>
       <c r="D46" s="1">
-        <v>104.9</v>
-      </c>
-      <c r="E46" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.6199999999999998E-2</v>
+        <v>98.92</v>
+      </c>
+      <c r="E46" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.3400000000000001E-2</v>
       </c>
       <c r="F46" s="1">
         <f>+((C46*$J$6)/$K$6)/1000</f>
-        <v>0.12801360000000001</v>
+        <v>0.15494419999999998</v>
       </c>
       <c r="G46" s="1">
         <f>+((D46*$J$6)/$K$6)/1000</f>
-        <v>0.11179342857142857</v>
+        <v>0.10542045714285715</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" s="1">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C47" s="1">
-        <v>118.49</v>
+        <v>120.12</v>
       </c>
       <c r="D47" s="1">
-        <v>104.36</v>
-      </c>
-      <c r="E47" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.7599999999999996E-2</v>
+        <v>98.11</v>
+      </c>
+      <c r="E47" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.3400000000000001E-2</v>
       </c>
       <c r="F47" s="1">
         <f>+((C47*$J$6)/$K$6)/1000</f>
-        <v>0.12627648571428571</v>
+        <v>0.12801360000000001</v>
       </c>
       <c r="G47" s="1">
         <f>+((D47*$J$6)/$K$6)/1000</f>
-        <v>0.11121794285714284</v>
+        <v>0.10455722857142857</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" s="1">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C48" s="1">
-        <v>122.56</v>
+        <v>132.35</v>
       </c>
       <c r="D48" s="1">
-        <v>103.81</v>
-      </c>
-      <c r="E48" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.1599999999999995E-2</v>
+        <v>81.8</v>
+      </c>
+      <c r="E48" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.3400000000000001E-2</v>
       </c>
       <c r="F48" s="1">
         <f>+((C48*$J$6)/$K$6)/1000</f>
-        <v>0.13061394285714284</v>
+        <v>0.14104728571428571</v>
       </c>
       <c r="G48" s="1">
         <f>+((D48*$J$6)/$K$6)/1000</f>
-        <v>0.1106318</v>
+        <v>8.717542857142857E-2</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C49" s="1">
-        <v>117.94</v>
+        <v>133.16</v>
       </c>
       <c r="D49" s="1">
-        <v>103.81</v>
-      </c>
-      <c r="E49" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.9000000000000002E-2</v>
+        <v>113.6</v>
+      </c>
+      <c r="E49" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.48E-2</v>
       </c>
       <c r="F49" s="1">
         <f>+((C49*$J$6)/$K$6)/1000</f>
-        <v>0.12569034285714284</v>
+        <v>0.14191051428571427</v>
       </c>
       <c r="G49" s="1">
         <f>+((D49*$J$6)/$K$6)/1000</f>
-        <v>0.1106318</v>
+        <v>0.12106514285714284</v>
       </c>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="1">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="C50" s="1">
-        <v>131.26</v>
+        <v>145.66</v>
       </c>
       <c r="D50" s="1">
-        <v>103.54</v>
-      </c>
-      <c r="E50" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.5799999999999997E-2</v>
+        <v>97.02</v>
+      </c>
+      <c r="E50" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.48E-2</v>
       </c>
       <c r="F50" s="1">
         <f>+((C50*$J$6)/$K$6)/1000</f>
-        <v>0.13988565714285714</v>
+        <v>0.15523194285714287</v>
       </c>
       <c r="G50" s="1">
         <f>+((D50*$J$6)/$K$6)/1000</f>
-        <v>0.11034405714285714</v>
+        <v>0.10339559999999999</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B51" s="1">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C51" s="1">
-        <v>145.66</v>
+        <v>118.49</v>
       </c>
       <c r="D51" s="1">
-        <v>103.54</v>
-      </c>
-      <c r="E51" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.7599999999999996E-2</v>
+        <v>95.93</v>
+      </c>
+      <c r="E51" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.48E-2</v>
       </c>
       <c r="F51" s="1">
         <f>+((C51*$J$6)/$K$6)/1000</f>
-        <v>0.15523194285714287</v>
+        <v>0.12627648571428571</v>
       </c>
       <c r="G51" s="1">
         <f>+((D51*$J$6)/$K$6)/1000</f>
-        <v>0.11034405714285714</v>
+        <v>0.10223397142857142</v>
       </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B52" s="1">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C52" s="1">
-        <v>118.49</v>
+        <v>133.97999999999999</v>
       </c>
       <c r="D52" s="1">
-        <v>103</v>
-      </c>
-      <c r="E52" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.1799999999999999E-2</v>
+        <v>81.260000000000005</v>
+      </c>
+      <c r="E52" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.48E-2</v>
       </c>
       <c r="F52" s="1">
         <f>+((C52*$J$6)/$K$6)/1000</f>
-        <v>0.12627648571428571</v>
+        <v>0.14278439999999998</v>
       </c>
       <c r="G52" s="1">
         <f>+((D52*$J$6)/$K$6)/1000</f>
-        <v>0.10976857142857142</v>
+        <v>8.659994285714287E-2</v>
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" s="1">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C53" s="1">
-        <v>122.29</v>
+        <v>135.07</v>
       </c>
       <c r="D53" s="1">
-        <v>103</v>
-      </c>
-      <c r="E53" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>3.6400000000000002E-2</v>
+        <v>114.96</v>
+      </c>
+      <c r="E53" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.6199999999999998E-2</v>
       </c>
       <c r="F53" s="1">
         <f>+((C53*$J$6)/$K$6)/1000</f>
-        <v>0.13032619999999998</v>
+        <v>0.14394602857142855</v>
       </c>
       <c r="G53" s="1">
         <f>+((D53*$J$6)/$K$6)/1000</f>
-        <v>0.10976857142857142</v>
+        <v>0.12251451428571429</v>
       </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B54" s="1">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C54" s="1">
-        <v>118.76</v>
+        <v>120.12</v>
       </c>
       <c r="D54" s="1">
-        <v>102.45</v>
-      </c>
-      <c r="E54" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.3199999999999997E-2</v>
+        <v>104.9</v>
+      </c>
+      <c r="E54" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.6199999999999998E-2</v>
       </c>
       <c r="F54" s="1">
         <f>+((C54*$J$6)/$K$6)/1000</f>
-        <v>0.12656422857142854</v>
+        <v>0.12801360000000001</v>
       </c>
       <c r="G54" s="1">
         <f>+((D54*$J$6)/$K$6)/1000</f>
-        <v>0.10918242857142856</v>
+        <v>0.11179342857142857</v>
       </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B55" s="1">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C55" s="1">
-        <v>117.94</v>
+        <v>113.87</v>
       </c>
       <c r="D55" s="1">
-        <v>102.18</v>
-      </c>
-      <c r="E55" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.6000000000000001E-2</v>
+        <v>97.83</v>
+      </c>
+      <c r="E55" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.6199999999999998E-2</v>
       </c>
       <c r="F55" s="1">
         <f>+((C55*$J$6)/$K$6)/1000</f>
-        <v>0.12569034285714284</v>
+        <v>0.12135288571428571</v>
       </c>
       <c r="G55" s="1">
         <f>+((D55*$J$6)/$K$6)/1000</f>
-        <v>0.10889468571428572</v>
+        <v>0.10425882857142857</v>
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B56" s="1">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C56" s="1">
-        <v>136.97</v>
+        <v>146.75</v>
       </c>
       <c r="D56" s="1">
-        <v>102.18</v>
-      </c>
-      <c r="E56" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>3.5000000000000003E-2</v>
+        <v>96.75</v>
+      </c>
+      <c r="E56" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.6199999999999998E-2</v>
       </c>
       <c r="F56" s="1">
         <f>+((C56*$J$6)/$K$6)/1000</f>
-        <v>0.14597088571428571</v>
+        <v>0.15639357142857141</v>
       </c>
       <c r="G56" s="1">
         <f>+((D56*$J$6)/$K$6)/1000</f>
-        <v>0.10889468571428572</v>
+        <v>0.10310785714285713</v>
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B57" s="1">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="C57" s="1">
-        <v>127.46</v>
+        <v>120.66</v>
       </c>
       <c r="D57" s="1">
-        <v>101.64</v>
-      </c>
-      <c r="E57" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.7199999999999982E-2</v>
+        <v>91.58</v>
+      </c>
+      <c r="E57" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.6199999999999998E-2</v>
       </c>
       <c r="F57" s="1">
         <f>+((C57*$J$6)/$K$6)/1000</f>
-        <v>0.13583594285714284</v>
+        <v>0.12858908571428568</v>
       </c>
       <c r="G57" s="1">
         <f>+((D57*$J$6)/$K$6)/1000</f>
-        <v>0.10831919999999998</v>
+        <v>9.7598114285714271E-2</v>
       </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B58" s="1">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C58" s="1">
-        <v>129.41</v>
+        <v>134.25</v>
       </c>
       <c r="D58" s="1">
-        <v>101.37</v>
-      </c>
-      <c r="E58" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>3.6400000000000002E-2</v>
+        <v>80.709999999999994</v>
+      </c>
+      <c r="E58" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.6199999999999998E-2</v>
       </c>
       <c r="F58" s="1">
         <f>+((C58*$J$6)/$K$6)/1000</f>
-        <v>0.13791408571428571</v>
+        <v>0.14307214285714284</v>
       </c>
       <c r="G58" s="1">
         <f>+((D58*$J$6)/$K$6)/1000</f>
-        <v>0.10803145714285714</v>
+        <v>8.6013799999999987E-2</v>
       </c>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59" s="1">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C59" s="1">
-        <v>117.4</v>
+        <v>133.97999999999999</v>
       </c>
       <c r="D59" s="1">
-        <v>100.28</v>
-      </c>
-      <c r="E59" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.74E-2</v>
+        <v>115.23</v>
+      </c>
+      <c r="E59" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.7599999999999996E-2</v>
       </c>
       <c r="F59" s="1">
         <f>+((C59*$J$6)/$K$6)/1000</f>
-        <v>0.12511485714285714</v>
+        <v>0.14278439999999998</v>
       </c>
       <c r="G59" s="1">
         <f>+((D59*$J$6)/$K$6)/1000</f>
-        <v>0.10686982857142857</v>
+        <v>0.12280225714285713</v>
       </c>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B60" s="1">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C60" s="1">
-        <v>118.22</v>
+        <v>118.49</v>
       </c>
       <c r="D60" s="1">
-        <v>100.01</v>
-      </c>
-      <c r="E60" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.8799999999999998E-2</v>
+        <v>104.36</v>
+      </c>
+      <c r="E60" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.7599999999999996E-2</v>
       </c>
       <c r="F60" s="1">
         <f>+((C60*$J$6)/$K$6)/1000</f>
-        <v>0.12598874285714284</v>
+        <v>0.12627648571428571</v>
       </c>
       <c r="G60" s="1">
         <f>+((D60*$J$6)/$K$6)/1000</f>
-        <v>0.10658208571428571</v>
+        <v>0.11121794285714284</v>
       </c>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B61" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C61" s="1">
-        <v>111.97</v>
+        <v>145.66</v>
       </c>
       <c r="D61" s="1">
-        <v>99.74</v>
-      </c>
-      <c r="E61" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.04E-2</v>
+        <v>103.54</v>
+      </c>
+      <c r="E61" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.7599999999999996E-2</v>
       </c>
       <c r="F61" s="1">
         <f>+((C61*$J$6)/$K$6)/1000</f>
-        <v>0.11932802857142856</v>
+        <v>0.15523194285714287</v>
       </c>
       <c r="G61" s="1">
         <f>+((D61*$J$6)/$K$6)/1000</f>
-        <v>0.10629434285714286</v>
+        <v>0.11034405714285714</v>
       </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B62" s="1">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C62" s="1">
-        <v>148.93</v>
+        <v>112.51</v>
       </c>
       <c r="D62" s="1">
-        <v>99.46</v>
-      </c>
-      <c r="E62" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.4599999999999996E-2</v>
+        <v>96.2</v>
+      </c>
+      <c r="E62" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.7599999999999996E-2</v>
       </c>
       <c r="F62" s="1">
         <f>+((C62*$J$6)/$K$6)/1000</f>
-        <v>0.15871682857142858</v>
+        <v>0.11990351428571427</v>
       </c>
       <c r="G62" s="1">
         <f>+((D62*$J$6)/$K$6)/1000</f>
-        <v>0.10599594285714284</v>
+        <v>0.10252171428571429</v>
       </c>
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B63" s="1">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C63" s="1">
-        <v>113.6</v>
+        <v>120.12</v>
       </c>
       <c r="D63" s="1">
-        <v>99.46</v>
-      </c>
-      <c r="E63" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.1799999999999999E-2</v>
+        <v>91.86</v>
+      </c>
+      <c r="E63" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.7599999999999996E-2</v>
       </c>
       <c r="F63" s="1">
         <f>+((C63*$J$6)/$K$6)/1000</f>
-        <v>0.12106514285714284</v>
+        <v>0.12801360000000001</v>
       </c>
       <c r="G63" s="1">
         <f>+((D63*$J$6)/$K$6)/1000</f>
-        <v>0.10599594285714284</v>
+        <v>9.7896514285714276E-2</v>
       </c>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B64" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C64" s="1">
-        <v>111.97</v>
+        <v>143.49</v>
       </c>
       <c r="D64" s="1">
-        <v>99.19</v>
-      </c>
-      <c r="E64" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.9000000000000002E-2</v>
+        <v>88.87</v>
+      </c>
+      <c r="E64" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.7599999999999996E-2</v>
       </c>
       <c r="F64" s="1">
         <f>+((C64*$J$6)/$K$6)/1000</f>
-        <v>0.11932802857142856</v>
+        <v>0.15291934285714284</v>
       </c>
       <c r="G64" s="1">
         <f>+((D64*$J$6)/$K$6)/1000</f>
-        <v>0.10570819999999999</v>
+        <v>9.4710028571428587E-2</v>
       </c>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B65" s="1">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C65" s="1">
-        <v>144.31</v>
+        <v>134.79</v>
       </c>
       <c r="D65" s="1">
-        <v>99.19</v>
-      </c>
-      <c r="E65" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.2000000000000003E-2</v>
+        <v>79.900000000000006</v>
+      </c>
+      <c r="E65" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.7599999999999996E-2</v>
       </c>
       <c r="F65" s="1">
         <f>+((C65*$J$6)/$K$6)/1000</f>
-        <v>0.15379322857142855</v>
+        <v>0.14364762857142854</v>
       </c>
       <c r="G65" s="1">
         <f>+((D65*$J$6)/$K$6)/1000</f>
-        <v>0.10570819999999999</v>
+        <v>8.5150571428571423E-2</v>
       </c>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B66" s="1">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C66" s="1">
-        <v>143.76</v>
+        <v>126.37</v>
       </c>
       <c r="D66" s="1">
-        <v>99.19</v>
-      </c>
-      <c r="E66" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>3.9199999999999999E-2</v>
+        <v>113.32</v>
+      </c>
+      <c r="E66" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="F66" s="1">
         <f>+((C66*$J$6)/$K$6)/1000</f>
-        <v>0.15320708571428571</v>
+        <v>0.13467431428571427</v>
       </c>
       <c r="G66" s="1">
         <f>+((D66*$J$6)/$K$6)/1000</f>
-        <v>0.10570819999999999</v>
+        <v>0.12076674285714284</v>
       </c>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67" s="1">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C67" s="1">
-        <v>145.38999999999999</v>
+        <v>139.96</v>
       </c>
       <c r="D67" s="1">
-        <v>98.92</v>
-      </c>
-      <c r="E67" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.3400000000000001E-2</v>
+        <v>110.88</v>
+      </c>
+      <c r="E67" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="F67" s="1">
         <f>+((C67*$J$6)/$K$6)/1000</f>
-        <v>0.15494419999999998</v>
+        <v>0.14915737142857141</v>
       </c>
       <c r="G67" s="1">
         <f>+((D67*$J$6)/$K$6)/1000</f>
-        <v>0.10542045714285715</v>
+        <v>0.11816639999999999</v>
       </c>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B68" s="1">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C68" s="1">
-        <v>139.41</v>
+        <v>117.94</v>
       </c>
       <c r="D68" s="1">
-        <v>98.92</v>
-      </c>
-      <c r="E68" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>3.6400000000000002E-2</v>
+        <v>103.81</v>
+      </c>
+      <c r="E68" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="F68" s="1">
         <f>+((C68*$J$6)/$K$6)/1000</f>
-        <v>0.14857122857142854</v>
+        <v>0.12569034285714284</v>
       </c>
       <c r="G68" s="1">
         <f>+((D68*$J$6)/$K$6)/1000</f>
-        <v>0.10542045714285715</v>
+        <v>0.1106318</v>
       </c>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B69" s="1">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C69" s="1">
-        <v>144.03</v>
+        <v>111.97</v>
       </c>
       <c r="D69" s="1">
-        <v>98.75</v>
-      </c>
-      <c r="E69" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.0599999999999997E-2</v>
+        <v>99.19</v>
+      </c>
+      <c r="E69" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="F69" s="1">
         <f>+((C69*$J$6)/$K$6)/1000</f>
-        <v>0.15349482857142857</v>
+        <v>0.11932802857142856</v>
       </c>
       <c r="G69" s="1">
         <f>+((D69*$J$6)/$K$6)/1000</f>
-        <v>0.1052392857142857</v>
+        <v>0.10570819999999999</v>
       </c>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B70" s="1">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C70" s="1">
-        <v>119.3</v>
+        <v>147.84</v>
       </c>
       <c r="D70" s="1">
-        <v>98.38</v>
-      </c>
-      <c r="E70" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.0199999999999997E-2</v>
+        <v>96.75</v>
+      </c>
+      <c r="E70" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="F70" s="1">
         <f>+((C70*$J$6)/$K$6)/1000</f>
-        <v>0.12713971428571427</v>
+        <v>0.15755519999999998</v>
       </c>
       <c r="G70" s="1">
         <f>+((D70*$J$6)/$K$6)/1000</f>
-        <v>0.10484497142857141</v>
+        <v>0.10310785714285713</v>
       </c>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B71" s="1">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C71" s="1">
-        <v>122.84</v>
+        <v>119.3</v>
       </c>
       <c r="D71" s="1">
-        <v>98.38</v>
-      </c>
-      <c r="E71" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>3.6400000000000002E-2</v>
+        <v>91.04</v>
+      </c>
+      <c r="E71" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="F71" s="1">
         <f>+((C71*$J$6)/$K$6)/1000</f>
-        <v>0.13091234285714284</v>
+        <v>0.12713971428571427</v>
       </c>
       <c r="G71" s="1">
         <f>+((D71*$J$6)/$K$6)/1000</f>
-        <v>0.10484497142857141</v>
+        <v>9.7022628571428571E-2</v>
       </c>
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B72" s="1">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C72" s="1">
-        <v>116.86</v>
+        <v>140.77000000000001</v>
       </c>
       <c r="D72" s="1">
-        <v>98.11</v>
-      </c>
-      <c r="E72" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.4599999999999996E-2</v>
+        <v>81.8</v>
+      </c>
+      <c r="E72" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="F72" s="1">
         <f>+((C72*$J$6)/$K$6)/1000</f>
-        <v>0.12453937142857141</v>
+        <v>0.15002059999999998</v>
       </c>
       <c r="G72" s="1">
         <f>+((D72*$J$6)/$K$6)/1000</f>
-        <v>0.10455722857142857</v>
+        <v>8.717542857142857E-2</v>
       </c>
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B73" s="1">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C73" s="1">
-        <v>148.65</v>
+        <v>130.44999999999999</v>
       </c>
       <c r="D73" s="1">
-        <v>98.11</v>
-      </c>
-      <c r="E73" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.3199999999999997E-2</v>
+        <v>80.709999999999994</v>
+      </c>
+      <c r="E73" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="F73" s="1">
         <f>+((C73*$J$6)/$K$6)/1000</f>
-        <v>0.15841842857142857</v>
+        <v>0.13902242857142855</v>
       </c>
       <c r="G73" s="1">
         <f>+((D73*$J$6)/$K$6)/1000</f>
-        <v>0.10455722857142857</v>
+        <v>8.6013799999999987E-2</v>
       </c>
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B74" s="1">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C74" s="1">
-        <v>120.12</v>
+        <v>139.69</v>
       </c>
       <c r="D74" s="1">
-        <v>98.11</v>
-      </c>
-      <c r="E74" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.3400000000000001E-2</v>
+        <v>113.87</v>
+      </c>
+      <c r="E74" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.04E-2</v>
       </c>
       <c r="F74" s="1">
         <f>+((C74*$J$6)/$K$6)/1000</f>
-        <v>0.12801360000000001</v>
+        <v>0.14886962857142857</v>
       </c>
       <c r="G74" s="1">
         <f>+((D74*$J$6)/$K$6)/1000</f>
-        <v>0.10455722857142857</v>
+        <v>0.12135288571428571</v>
       </c>
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B75" s="1">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C75" s="1">
-        <v>121.21</v>
+        <v>125.09</v>
       </c>
       <c r="D75" s="1">
-        <v>98.11</v>
-      </c>
-      <c r="E75" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.0599999999999997E-2</v>
+        <v>112.7</v>
+      </c>
+      <c r="E75" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.04E-2</v>
       </c>
       <c r="F75" s="1">
         <f>+((C75*$J$6)/$K$6)/1000</f>
-        <v>0.12917522857142857</v>
+        <v>0.13331020000000002</v>
       </c>
       <c r="G75" s="1">
         <f>+((D75*$J$6)/$K$6)/1000</f>
-        <v>0.10455722857142857</v>
+        <v>0.12010599999999999</v>
       </c>
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B76" s="1">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C76" s="1">
-        <v>141.59</v>
+        <v>119.85</v>
       </c>
       <c r="D76" s="1">
-        <v>98.11</v>
-      </c>
-      <c r="E76" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>3.78E-2</v>
+        <v>104.9</v>
+      </c>
+      <c r="E76" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.04E-2</v>
       </c>
       <c r="F76" s="1">
         <f>+((C76*$J$6)/$K$6)/1000</f>
-        <v>0.15089448571428571</v>
+        <v>0.12772585714285714</v>
       </c>
       <c r="G76" s="1">
         <f>+((D76*$J$6)/$K$6)/1000</f>
-        <v>0.10455722857142857</v>
+        <v>0.11179342857142857</v>
       </c>
     </row>
     <row r="77" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B77" s="1">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C77" s="1">
-        <v>121.21</v>
+        <v>111.97</v>
       </c>
       <c r="D77" s="1">
-        <v>98.11</v>
-      </c>
-      <c r="E77" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>3.78E-2</v>
+        <v>99.74</v>
+      </c>
+      <c r="E77" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.04E-2</v>
       </c>
       <c r="F77" s="1">
         <f>+((C77*$J$6)/$K$6)/1000</f>
-        <v>0.12917522857142857</v>
+        <v>0.11932802857142856</v>
       </c>
       <c r="G77" s="1">
         <f>+((D77*$J$6)/$K$6)/1000</f>
-        <v>0.10455722857142857</v>
+        <v>0.10629434285714286</v>
       </c>
     </row>
     <row r="78" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B78" s="1">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C78" s="1">
-        <v>136.41999999999999</v>
+        <v>147.84</v>
       </c>
       <c r="D78" s="1">
-        <v>98.11</v>
-      </c>
-      <c r="E78" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>3.3599999999999991E-2</v>
+        <v>95.66</v>
+      </c>
+      <c r="E78" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.04E-2</v>
       </c>
       <c r="F78" s="1">
         <f>+((C78*$J$6)/$K$6)/1000</f>
-        <v>0.14538474285714284</v>
+        <v>0.15755519999999998</v>
       </c>
       <c r="G78" s="1">
         <f>+((D78*$J$6)/$K$6)/1000</f>
-        <v>0.10455722857142857</v>
+        <v>0.10194622857142856</v>
       </c>
     </row>
     <row r="79" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B79" s="1">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C79" s="1">
-        <v>146.47999999999999</v>
+        <v>119.03</v>
       </c>
       <c r="D79" s="1">
-        <v>97.83</v>
-      </c>
-      <c r="E79" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.1599999999999995E-2</v>
+        <v>91.87</v>
+      </c>
+      <c r="E79" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.04E-2</v>
       </c>
       <c r="F79" s="1">
         <f>+((C79*$J$6)/$K$6)/1000</f>
-        <v>0.15610582857142855</v>
+        <v>0.12685197142857141</v>
       </c>
       <c r="G79" s="1">
         <f>+((D79*$J$6)/$K$6)/1000</f>
-        <v>0.10425882857142857</v>
+        <v>9.7907171428571416E-2</v>
       </c>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B80" s="1">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C80" s="1">
-        <v>113.87</v>
+        <v>133.71</v>
       </c>
       <c r="D80" s="1">
-        <v>97.83</v>
-      </c>
-      <c r="E80" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.6199999999999998E-2</v>
+        <v>80.17</v>
+      </c>
+      <c r="E80" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.04E-2</v>
       </c>
       <c r="F80" s="1">
         <f>+((C80*$J$6)/$K$6)/1000</f>
-        <v>0.12135288571428571</v>
+        <v>0.14249665714285714</v>
       </c>
       <c r="G80" s="1">
         <f>+((D80*$J$6)/$K$6)/1000</f>
-        <v>0.10425882857142857</v>
+        <v>8.5438314285714287E-2</v>
       </c>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B81" s="1">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C81" s="1">
-        <v>121.21</v>
+        <v>125.55</v>
       </c>
       <c r="D81" s="1">
-        <v>97.83</v>
-      </c>
-      <c r="E81" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>3.9199999999999999E-2</v>
+        <v>114.14</v>
+      </c>
+      <c r="E81" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.1799999999999999E-2</v>
       </c>
       <c r="F81" s="1">
         <f>+((C81*$J$6)/$K$6)/1000</f>
-        <v>0.12917522857142857</v>
+        <v>0.13380042857142857</v>
       </c>
       <c r="G81" s="1">
         <f>+((D81*$J$6)/$K$6)/1000</f>
-        <v>0.10425882857142857</v>
+        <v>0.12164062857142856</v>
       </c>
     </row>
     <row r="82" spans="2:7" x14ac:dyDescent="0.25">
@@ -2332,597 +2348,597 @@
         <v>37</v>
       </c>
       <c r="C82" s="1">
-        <v>148.38</v>
+        <v>142.13</v>
       </c>
       <c r="D82" s="1">
-        <v>97.56</v>
-      </c>
-      <c r="E82" s="7">
+        <v>109.79</v>
+      </c>
+      <c r="E82" s="6">
         <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
         <v>5.1799999999999999E-2</v>
       </c>
       <c r="F82" s="1">
         <f>+((C82*$J$6)/$K$6)/1000</f>
-        <v>0.15813068571428571</v>
+        <v>0.15146997142857144</v>
       </c>
       <c r="G82" s="1">
         <f>+((D82*$J$6)/$K$6)/1000</f>
-        <v>0.1039710857142857</v>
+        <v>0.11700477142857144</v>
       </c>
     </row>
     <row r="83" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B83" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C83" s="1">
-        <v>114.68</v>
+        <v>118.49</v>
       </c>
       <c r="D83" s="1">
-        <v>97.29</v>
-      </c>
-      <c r="E83" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.3199999999999997E-2</v>
+        <v>103</v>
+      </c>
+      <c r="E83" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.1799999999999999E-2</v>
       </c>
       <c r="F83" s="1">
         <f>+((C83*$J$6)/$K$6)/1000</f>
-        <v>0.1222161142857143</v>
+        <v>0.12627648571428571</v>
       </c>
       <c r="G83" s="1">
         <f>+((D83*$J$6)/$K$6)/1000</f>
-        <v>0.10368334285714285</v>
+        <v>0.10976857142857142</v>
       </c>
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B84" s="1">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="C84" s="1">
-        <v>125.83</v>
+        <v>113.6</v>
       </c>
       <c r="D84" s="1">
-        <v>97.29</v>
-      </c>
-      <c r="E84" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>3.3599999999999991E-2</v>
+        <v>99.46</v>
+      </c>
+      <c r="E84" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.1799999999999999E-2</v>
       </c>
       <c r="F84" s="1">
         <f>+((C84*$J$6)/$K$6)/1000</f>
-        <v>0.13409882857142855</v>
+        <v>0.12106514285714284</v>
       </c>
       <c r="G84" s="1">
         <f>+((D84*$J$6)/$K$6)/1000</f>
-        <v>0.10368334285714285</v>
+        <v>0.10599594285714284</v>
       </c>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B85" s="1">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C85" s="1">
-        <v>145.66</v>
+        <v>148.38</v>
       </c>
       <c r="D85" s="1">
-        <v>97.02</v>
-      </c>
-      <c r="E85" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.48E-2</v>
+        <v>97.56</v>
+      </c>
+      <c r="E85" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.1799999999999999E-2</v>
       </c>
       <c r="F85" s="1">
         <f>+((C85*$J$6)/$K$6)/1000</f>
-        <v>0.15523194285714287</v>
+        <v>0.15813068571428571</v>
       </c>
       <c r="G85" s="1">
         <f>+((D85*$J$6)/$K$6)/1000</f>
-        <v>0.10339559999999999</v>
+        <v>0.1039710857142857</v>
       </c>
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B86" s="1">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C86" s="1">
-        <v>120.12</v>
+        <v>118.76</v>
       </c>
       <c r="D86" s="1">
-        <v>97.02</v>
-      </c>
-      <c r="E86" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.2000000000000003E-2</v>
+        <v>92.4</v>
+      </c>
+      <c r="E86" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.1799999999999999E-2</v>
       </c>
       <c r="F86" s="1">
         <f>+((C86*$J$6)/$K$6)/1000</f>
-        <v>0.12801360000000001</v>
+        <v>0.12656422857142854</v>
       </c>
       <c r="G86" s="1">
         <f>+((D86*$J$6)/$K$6)/1000</f>
-        <v>0.10339559999999999</v>
+        <v>9.847199999999999E-2</v>
       </c>
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B87" s="1">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C87" s="1">
-        <v>146.75</v>
+        <v>133.71</v>
       </c>
       <c r="D87" s="1">
-        <v>96.75</v>
-      </c>
-      <c r="E87" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.0199999999999997E-2</v>
+        <v>80.44</v>
+      </c>
+      <c r="E87" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.1799999999999999E-2</v>
       </c>
       <c r="F87" s="1">
         <f>+((C87*$J$6)/$K$6)/1000</f>
-        <v>0.15639357142857141</v>
+        <v>0.14249665714285714</v>
       </c>
       <c r="G87" s="1">
         <f>+((D87*$J$6)/$K$6)/1000</f>
-        <v>0.10310785714285713</v>
+        <v>8.5726057142857137E-2</v>
       </c>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B88" s="1">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C88" s="1">
-        <v>147.84</v>
+        <v>126.37</v>
       </c>
       <c r="D88" s="1">
-        <v>96.75</v>
-      </c>
-      <c r="E88" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.9000000000000002E-2</v>
+        <v>114.96</v>
+      </c>
+      <c r="E88" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.3199999999999997E-2</v>
       </c>
       <c r="F88" s="1">
         <f>+((C88*$J$6)/$K$6)/1000</f>
-        <v>0.15755519999999998</v>
+        <v>0.13467431428571427</v>
       </c>
       <c r="G88" s="1">
         <f>+((D88*$J$6)/$K$6)/1000</f>
-        <v>0.10310785714285713</v>
+        <v>0.12251451428571429</v>
       </c>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B89" s="1">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C89" s="1">
-        <v>146.75</v>
+        <v>140.22999999999999</v>
       </c>
       <c r="D89" s="1">
-        <v>96.75</v>
-      </c>
-      <c r="E89" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.6199999999999998E-2</v>
+        <v>113.6</v>
+      </c>
+      <c r="E89" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.3199999999999997E-2</v>
       </c>
       <c r="F89" s="1">
         <f>+((C89*$J$6)/$K$6)/1000</f>
-        <v>0.15639357142857141</v>
+        <v>0.14944511428571425</v>
       </c>
       <c r="G89" s="1">
         <f>+((D89*$J$6)/$K$6)/1000</f>
-        <v>0.10310785714285713</v>
+        <v>0.12106514285714284</v>
       </c>
     </row>
     <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B90" s="1">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C90" s="1">
-        <v>142.94999999999999</v>
+        <v>118.76</v>
       </c>
       <c r="D90" s="1">
-        <v>96.2</v>
-      </c>
-      <c r="E90" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.4399999999999985E-2</v>
+        <v>102.45</v>
+      </c>
+      <c r="E90" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.3199999999999997E-2</v>
       </c>
       <c r="F90" s="1">
         <f>+((C90*$J$6)/$K$6)/1000</f>
-        <v>0.15234385714285711</v>
+        <v>0.12656422857142854</v>
       </c>
       <c r="G90" s="1">
         <f>+((D90*$J$6)/$K$6)/1000</f>
-        <v>0.10252171428571429</v>
+        <v>0.10918242857142856</v>
       </c>
     </row>
     <row r="91" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B91" s="1">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C91" s="1">
-        <v>112.51</v>
+        <v>148.65</v>
       </c>
       <c r="D91" s="1">
-        <v>96.2</v>
-      </c>
-      <c r="E91" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.7599999999999996E-2</v>
+        <v>98.11</v>
+      </c>
+      <c r="E91" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.3199999999999997E-2</v>
       </c>
       <c r="F91" s="1">
         <f>+((C91*$J$6)/$K$6)/1000</f>
-        <v>0.11990351428571427</v>
+        <v>0.15841842857142857</v>
       </c>
       <c r="G91" s="1">
         <f>+((D91*$J$6)/$K$6)/1000</f>
-        <v>0.10252171428571429</v>
+        <v>0.10455722857142857</v>
       </c>
     </row>
     <row r="92" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B92" s="1">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C92" s="1">
-        <v>138.33000000000001</v>
+        <v>114.68</v>
       </c>
       <c r="D92" s="1">
-        <v>95.93</v>
-      </c>
-      <c r="E92" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.5799999999999997E-2</v>
+        <v>97.29</v>
+      </c>
+      <c r="E92" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.3199999999999997E-2</v>
       </c>
       <c r="F92" s="1">
         <f>+((C92*$J$6)/$K$6)/1000</f>
-        <v>0.14742025714285714</v>
+        <v>0.1222161142857143</v>
       </c>
       <c r="G92" s="1">
         <f>+((D92*$J$6)/$K$6)/1000</f>
-        <v>0.10223397142857142</v>
+        <v>0.10368334285714285</v>
       </c>
     </row>
     <row r="93" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B93" s="1">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C93" s="1">
-        <v>118.49</v>
+        <v>118.22</v>
       </c>
       <c r="D93" s="1">
-        <v>95.93</v>
-      </c>
-      <c r="E93" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.48E-2</v>
+        <v>93.21</v>
+      </c>
+      <c r="E93" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.3199999999999997E-2</v>
       </c>
       <c r="F93" s="1">
         <f>+((C93*$J$6)/$K$6)/1000</f>
-        <v>0.12627648571428571</v>
+        <v>0.12598874285714284</v>
       </c>
       <c r="G93" s="1">
         <f>+((D93*$J$6)/$K$6)/1000</f>
-        <v>0.10223397142857142</v>
+        <v>9.9335228571428555E-2</v>
       </c>
     </row>
     <row r="94" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B94" s="1">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C94" s="1">
-        <v>147.84</v>
+        <v>123.38</v>
       </c>
       <c r="D94" s="1">
-        <v>95.66</v>
-      </c>
-      <c r="E94" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.04E-2</v>
+        <v>82.62</v>
+      </c>
+      <c r="E94" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.3199999999999997E-2</v>
       </c>
       <c r="F94" s="1">
         <f>+((C94*$J$6)/$K$6)/1000</f>
-        <v>0.15755519999999998</v>
+        <v>0.13148782857142857</v>
       </c>
       <c r="G94" s="1">
         <f>+((D94*$J$6)/$K$6)/1000</f>
-        <v>0.10194622857142856</v>
+        <v>8.8049314285714289E-2</v>
       </c>
     </row>
     <row r="95" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B95" s="1">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C95" s="1">
-        <v>144.85</v>
+        <v>138.6</v>
       </c>
       <c r="D95" s="1">
-        <v>95.39</v>
-      </c>
-      <c r="E95" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.2999999999999987E-2</v>
+        <v>81.8</v>
+      </c>
+      <c r="E95" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.3199999999999997E-2</v>
       </c>
       <c r="F95" s="1">
         <f>+((C95*$J$6)/$K$6)/1000</f>
-        <v>0.15436871428571428</v>
+        <v>0.14770800000000001</v>
       </c>
       <c r="G95" s="1">
         <f>+((D95*$J$6)/$K$6)/1000</f>
-        <v>0.10165848571428571</v>
+        <v>8.717542857142857E-2</v>
       </c>
     </row>
     <row r="96" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B96" s="1">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C96" s="1">
-        <v>124.27</v>
+        <v>128.82</v>
       </c>
       <c r="D96" s="1">
-        <v>95.39</v>
-      </c>
-      <c r="E96" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>3.5000000000000003E-2</v>
+        <v>80.989999999999995</v>
+      </c>
+      <c r="E96" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.3199999999999997E-2</v>
       </c>
       <c r="F96" s="1">
         <f>+((C96*$J$6)/$K$6)/1000</f>
-        <v>0.13243631428571428</v>
+        <v>0.13728531428571428</v>
       </c>
       <c r="G96" s="1">
         <f>+((D96*$J$6)/$K$6)/1000</f>
-        <v>0.10165848571428571</v>
+        <v>8.6312199999999992E-2</v>
       </c>
     </row>
     <row r="97" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B97" s="1">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="C97" s="1">
-        <v>123.65</v>
+        <v>125.01</v>
       </c>
       <c r="D97" s="1">
-        <v>95.2</v>
-      </c>
-      <c r="E97" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>3.6400000000000002E-2</v>
+        <v>114.14</v>
+      </c>
+      <c r="E97" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.4599999999999996E-2</v>
       </c>
       <c r="F97" s="1">
         <f>+((C97*$J$6)/$K$6)/1000</f>
-        <v>0.13177557142857144</v>
+        <v>0.13322494285714284</v>
       </c>
       <c r="G97" s="1">
         <f>+((D97*$J$6)/$K$6)/1000</f>
-        <v>0.101456</v>
+        <v>0.12164062857142856</v>
       </c>
     </row>
     <row r="98" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B98" s="1">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C98" s="1">
-        <v>120.93</v>
+        <v>140.22999999999999</v>
       </c>
       <c r="D98" s="1">
-        <v>94.85</v>
-      </c>
-      <c r="E98" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.4399999999999985E-2</v>
+        <v>113.6</v>
+      </c>
+      <c r="E98" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.4599999999999996E-2</v>
       </c>
       <c r="F98" s="1">
         <f>+((C98*$J$6)/$K$6)/1000</f>
-        <v>0.12887682857142857</v>
+        <v>0.14944511428571425</v>
       </c>
       <c r="G98" s="1">
         <f>+((D98*$J$6)/$K$6)/1000</f>
-        <v>0.10108299999999999</v>
+        <v>0.12106514285714284</v>
       </c>
     </row>
     <row r="99" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B99" s="1">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="C99" s="1">
-        <v>135.34</v>
+        <v>148.93</v>
       </c>
       <c r="D99" s="1">
-        <v>94.85</v>
-      </c>
-      <c r="E99" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>3.5000000000000003E-2</v>
+        <v>99.46</v>
+      </c>
+      <c r="E99" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.4599999999999996E-2</v>
       </c>
       <c r="F99" s="1">
         <f>+((C99*$J$6)/$K$6)/1000</f>
-        <v>0.14423377142857144</v>
+        <v>0.15871682857142858</v>
       </c>
       <c r="G99" s="1">
         <f>+((D99*$J$6)/$K$6)/1000</f>
-        <v>0.10108299999999999</v>
+        <v>0.10599594285714284</v>
       </c>
     </row>
     <row r="100" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B100" s="1">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C100" s="1">
-        <v>136.15</v>
+        <v>116.86</v>
       </c>
       <c r="D100" s="1">
-        <v>94.57</v>
-      </c>
-      <c r="E100" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.7199999999999982E-2</v>
+        <v>98.11</v>
+      </c>
+      <c r="E100" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.4599999999999996E-2</v>
       </c>
       <c r="F100" s="1">
         <f>+((C100*$J$6)/$K$6)/1000</f>
-        <v>0.14509699999999998</v>
+        <v>0.12453937142857141</v>
       </c>
       <c r="G100" s="1">
         <f>+((D100*$J$6)/$K$6)/1000</f>
-        <v>0.10078459999999999</v>
+        <v>0.10455722857142857</v>
       </c>
     </row>
     <row r="101" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B101" s="1">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C101" s="1">
-        <v>123.38</v>
+        <v>142.68</v>
       </c>
       <c r="D101" s="1">
-        <v>94.03</v>
-      </c>
-      <c r="E101" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.5799999999999997E-2</v>
+        <v>88.59</v>
+      </c>
+      <c r="E101" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.4599999999999996E-2</v>
       </c>
       <c r="F101" s="1">
         <f>+((C101*$J$6)/$K$6)/1000</f>
-        <v>0.13148782857142857</v>
+        <v>0.15205611428571428</v>
       </c>
       <c r="G101" s="1">
         <f>+((D101*$J$6)/$K$6)/1000</f>
-        <v>0.10020911428571427</v>
+        <v>9.4411628571428569E-2</v>
       </c>
     </row>
     <row r="102" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B102" s="1">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="C102" s="1">
-        <v>137.24</v>
+        <v>123.38</v>
       </c>
       <c r="D102" s="1">
-        <v>94.03</v>
-      </c>
-      <c r="E102" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>3.6400000000000002E-2</v>
+        <v>82.62</v>
+      </c>
+      <c r="E102" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.4599999999999996E-2</v>
       </c>
       <c r="F102" s="1">
         <f>+((C102*$J$6)/$K$6)/1000</f>
-        <v>0.14625862857142857</v>
+        <v>0.13148782857142857</v>
       </c>
       <c r="G102" s="1">
         <f>+((D102*$J$6)/$K$6)/1000</f>
-        <v>0.10020911428571427</v>
+        <v>8.8049314285714289E-2</v>
       </c>
     </row>
     <row r="103" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B103" s="1">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C103" s="1">
-        <v>147.02000000000001</v>
+        <v>132.88999999999999</v>
       </c>
       <c r="D103" s="1">
-        <v>93.21</v>
-      </c>
-      <c r="E103" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.74E-2</v>
+        <v>80.989999999999995</v>
+      </c>
+      <c r="E103" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.4599999999999996E-2</v>
       </c>
       <c r="F103" s="1">
         <f>+((C103*$J$6)/$K$6)/1000</f>
-        <v>0.15668131428571427</v>
+        <v>0.14162277142857138</v>
       </c>
       <c r="G103" s="1">
         <f>+((D103*$J$6)/$K$6)/1000</f>
-        <v>9.9335228571428555E-2</v>
+        <v>8.6312199999999992E-2</v>
       </c>
     </row>
     <row r="104" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B104" s="1">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C104" s="1">
-        <v>118.22</v>
+        <v>139.96</v>
       </c>
       <c r="D104" s="1">
-        <v>93.21</v>
-      </c>
-      <c r="E104" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.3199999999999997E-2</v>
+        <v>113.6</v>
+      </c>
+      <c r="E104" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="F104" s="1">
         <f>+((C104*$J$6)/$K$6)/1000</f>
-        <v>0.12598874285714284</v>
+        <v>0.14915737142857141</v>
       </c>
       <c r="G104" s="1">
         <f>+((D104*$J$6)/$K$6)/1000</f>
-        <v>9.9335228571428555E-2</v>
+        <v>0.12106514285714284</v>
       </c>
     </row>
     <row r="105" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B105" s="1">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C105" s="1">
-        <v>120.66</v>
+        <v>124.74</v>
       </c>
       <c r="D105" s="1">
-        <v>92.67</v>
-      </c>
-      <c r="E105" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.2999999999999987E-2</v>
+        <v>112.51</v>
+      </c>
+      <c r="E105" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="F105" s="1">
         <f>+((C105*$J$6)/$K$6)/1000</f>
-        <v>0.12858908571428568</v>
+        <v>0.13293719999999998</v>
       </c>
       <c r="G105" s="1">
         <f>+((D105*$J$6)/$K$6)/1000</f>
-        <v>9.8759742857142854E-2</v>
+        <v>0.11990351428571427</v>
       </c>
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B106" s="1">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C106" s="1">
-        <v>118.76</v>
+        <v>145.38999999999999</v>
       </c>
       <c r="D106" s="1">
-        <v>92.4</v>
-      </c>
-      <c r="E106" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.1799999999999999E-2</v>
+        <v>105.72</v>
+      </c>
+      <c r="E106" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="F106" s="1">
         <f>+((C106*$J$6)/$K$6)/1000</f>
-        <v>0.12656422857142854</v>
+        <v>0.15494419999999998</v>
       </c>
       <c r="G106" s="1">
         <f>+((D106*$J$6)/$K$6)/1000</f>
-        <v>9.847199999999999E-2</v>
+        <v>0.11266731428571429</v>
       </c>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B107" s="1">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C107" s="1">
-        <v>123.92</v>
+        <v>117.94</v>
       </c>
       <c r="D107" s="1">
-        <v>92.13</v>
-      </c>
-      <c r="E107" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.7199999999999982E-2</v>
+        <v>102.18</v>
+      </c>
+      <c r="E107" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="F107" s="1">
         <f>+((C107*$J$6)/$K$6)/1000</f>
-        <v>0.13206331428571425</v>
+        <v>0.12569034285714284</v>
       </c>
       <c r="G107" s="1">
         <f>+((D107*$J$6)/$K$6)/1000</f>
-        <v>9.818425714285714E-2</v>
+        <v>0.10889468571428572</v>
       </c>
     </row>
     <row r="108" spans="2:7" x14ac:dyDescent="0.25">
@@ -2935,7 +2951,7 @@
       <c r="D108" s="1">
         <v>92.13</v>
       </c>
-      <c r="E108" s="7">
+      <c r="E108" s="6">
         <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
         <v>5.6000000000000001E-2</v>
       </c>
@@ -2950,439 +2966,439 @@
     </row>
     <row r="109" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B109" s="1">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C109" s="1">
-        <v>119.03</v>
+        <v>118.49</v>
       </c>
       <c r="D109" s="1">
-        <v>91.87</v>
-      </c>
-      <c r="E109" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.04E-2</v>
+        <v>88.32</v>
+      </c>
+      <c r="E109" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="F109" s="1">
         <f>+((C109*$J$6)/$K$6)/1000</f>
-        <v>0.12685197142857141</v>
+        <v>0.12627648571428571</v>
       </c>
       <c r="G109" s="1">
         <f>+((D109*$J$6)/$K$6)/1000</f>
-        <v>9.7907171428571416E-2</v>
+        <v>9.4123885714285691E-2</v>
       </c>
     </row>
     <row r="110" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B110" s="1">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C110" s="1">
-        <v>120.12</v>
+        <v>139.41</v>
       </c>
       <c r="D110" s="1">
-        <v>91.86</v>
-      </c>
-      <c r="E110" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.7599999999999996E-2</v>
+        <v>83.7</v>
+      </c>
+      <c r="E110" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="F110" s="1">
         <f>+((C110*$J$6)/$K$6)/1000</f>
-        <v>0.12801360000000001</v>
+        <v>0.14857122857142854</v>
       </c>
       <c r="G110" s="1">
         <f>+((D110*$J$6)/$K$6)/1000</f>
-        <v>9.7896514285714276E-2</v>
+        <v>8.9200285714285718E-2</v>
       </c>
     </row>
     <row r="111" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B111" s="1">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C111" s="1">
-        <v>145.66</v>
+        <v>125.83</v>
       </c>
       <c r="D111" s="1">
-        <v>91.58</v>
-      </c>
-      <c r="E111" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.8799999999999998E-2</v>
+        <v>81.53</v>
+      </c>
+      <c r="E111" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="F111" s="1">
         <f>+((C111*$J$6)/$K$6)/1000</f>
-        <v>0.15523194285714287</v>
+        <v>0.13409882857142855</v>
       </c>
       <c r="G111" s="1">
         <f>+((D111*$J$6)/$K$6)/1000</f>
-        <v>9.7598114285714271E-2</v>
+        <v>8.6887685714285706E-2</v>
       </c>
     </row>
     <row r="112" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B112" s="1">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C112" s="1">
-        <v>120.66</v>
+        <v>137.51</v>
       </c>
       <c r="D112" s="1">
-        <v>91.58</v>
-      </c>
-      <c r="E112" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.6199999999999998E-2</v>
+        <v>113.05</v>
+      </c>
+      <c r="E112" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.74E-2</v>
       </c>
       <c r="F112" s="1">
         <f>+((C112*$J$6)/$K$6)/1000</f>
-        <v>0.12858908571428568</v>
+        <v>0.14654637142857141</v>
       </c>
       <c r="G112" s="1">
         <f>+((D112*$J$6)/$K$6)/1000</f>
-        <v>9.7598114285714271E-2</v>
+        <v>0.12047899999999999</v>
       </c>
     </row>
     <row r="113" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B113" s="1">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="C113" s="1">
-        <v>130.44999999999999</v>
+        <v>126.1</v>
       </c>
       <c r="D113" s="1">
-        <v>91.31</v>
-      </c>
-      <c r="E113" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>3.3599999999999991E-2</v>
+        <v>113.05</v>
+      </c>
+      <c r="E113" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.74E-2</v>
       </c>
       <c r="F113" s="1">
         <f>+((C113*$J$6)/$K$6)/1000</f>
-        <v>0.13902242857142855</v>
+        <v>0.13438657142857141</v>
       </c>
       <c r="G113" s="1">
         <f>+((D113*$J$6)/$K$6)/1000</f>
-        <v>9.7310371428571435E-2</v>
+        <v>0.12047899999999999</v>
       </c>
     </row>
     <row r="114" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B114" s="1">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C114" s="1">
-        <v>119.3</v>
+        <v>144.85</v>
       </c>
       <c r="D114" s="1">
-        <v>91.04</v>
-      </c>
-      <c r="E114" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.9000000000000002E-2</v>
+        <v>105.72</v>
+      </c>
+      <c r="E114" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.74E-2</v>
       </c>
       <c r="F114" s="1">
         <f>+((C114*$J$6)/$K$6)/1000</f>
-        <v>0.12713971428571427</v>
+        <v>0.15436871428571428</v>
       </c>
       <c r="G114" s="1">
         <f>+((D114*$J$6)/$K$6)/1000</f>
-        <v>9.7022628571428571E-2</v>
+        <v>0.11266731428571429</v>
       </c>
     </row>
     <row r="115" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B115" s="1">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C115" s="1">
-        <v>137.24</v>
+        <v>117.4</v>
       </c>
       <c r="D115" s="1">
-        <v>90.77</v>
-      </c>
-      <c r="E115" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.4399999999999985E-2</v>
+        <v>100.28</v>
+      </c>
+      <c r="E115" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.74E-2</v>
       </c>
       <c r="F115" s="1">
         <f>+((C115*$J$6)/$K$6)/1000</f>
-        <v>0.14625862857142857</v>
+        <v>0.12511485714285714</v>
       </c>
       <c r="G115" s="1">
         <f>+((D115*$J$6)/$K$6)/1000</f>
-        <v>9.6734885714285693E-2</v>
+        <v>0.10686982857142857</v>
       </c>
     </row>
     <row r="116" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B116" s="1">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C116" s="1">
-        <v>119.58</v>
+        <v>147.02000000000001</v>
       </c>
       <c r="D116" s="1">
-        <v>90.77</v>
-      </c>
-      <c r="E116" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.1599999999999995E-2</v>
+        <v>93.21</v>
+      </c>
+      <c r="E116" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.74E-2</v>
       </c>
       <c r="F116" s="1">
         <f>+((C116*$J$6)/$K$6)/1000</f>
-        <v>0.12743811428571428</v>
+        <v>0.15668131428571427</v>
       </c>
       <c r="G116" s="1">
         <f>+((D116*$J$6)/$K$6)/1000</f>
-        <v>9.6734885714285693E-2</v>
+        <v>9.9335228571428555E-2</v>
       </c>
     </row>
     <row r="117" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B117" s="1">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="C117" s="1">
-        <v>129.09</v>
+        <v>120.12</v>
       </c>
       <c r="D117" s="1">
-        <v>90.5</v>
-      </c>
-      <c r="E117" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>3.5000000000000003E-2</v>
+        <v>87.24</v>
+      </c>
+      <c r="E117" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.74E-2</v>
       </c>
       <c r="F117" s="1">
         <f>+((C117*$J$6)/$K$6)/1000</f>
-        <v>0.13757305714285711</v>
+        <v>0.12801360000000001</v>
       </c>
       <c r="G117" s="1">
         <f>+((D117*$J$6)/$K$6)/1000</f>
-        <v>9.6447142857142856E-2</v>
+        <v>9.2972914285714275E-2</v>
       </c>
     </row>
     <row r="118" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B118" s="1">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="C118" s="1">
-        <v>128.54</v>
+        <v>138.33000000000001</v>
       </c>
       <c r="D118" s="1">
-        <v>89.14</v>
-      </c>
-      <c r="E118" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>3.6400000000000002E-2</v>
+        <v>83.43</v>
+      </c>
+      <c r="E118" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.74E-2</v>
       </c>
       <c r="F118" s="1">
         <f>+((C118*$J$6)/$K$6)/1000</f>
-        <v>0.13698691428571427</v>
+        <v>0.14742025714285714</v>
       </c>
       <c r="G118" s="1">
         <f>+((D118*$J$6)/$K$6)/1000</f>
-        <v>9.4997771428571409E-2</v>
+        <v>8.8912542857142854E-2</v>
       </c>
     </row>
     <row r="119" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B119" s="1">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C119" s="1">
-        <v>143.49</v>
+        <v>125.28</v>
       </c>
       <c r="D119" s="1">
-        <v>88.87</v>
-      </c>
-      <c r="E119" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.7599999999999996E-2</v>
+        <v>82.34</v>
+      </c>
+      <c r="E119" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.74E-2</v>
       </c>
       <c r="F119" s="1">
         <f>+((C119*$J$6)/$K$6)/1000</f>
-        <v>0.15291934285714284</v>
+        <v>0.13351268571428571</v>
       </c>
       <c r="G119" s="1">
         <f>+((D119*$J$6)/$K$6)/1000</f>
-        <v>9.4710028571428587E-2</v>
+        <v>8.7750914285714271E-2</v>
       </c>
     </row>
     <row r="120" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B120" s="1">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C120" s="1">
-        <v>130.16999999999999</v>
+        <v>129.09</v>
       </c>
       <c r="D120" s="1">
-        <v>88.87</v>
-      </c>
-      <c r="E120" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>3.6400000000000002E-2</v>
+        <v>113.05</v>
+      </c>
+      <c r="E120" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.8799999999999998E-2</v>
       </c>
       <c r="F120" s="1">
         <f>+((C120*$J$6)/$K$6)/1000</f>
-        <v>0.13872402857142857</v>
+        <v>0.13757305714285711</v>
       </c>
       <c r="G120" s="1">
         <f>+((D120*$J$6)/$K$6)/1000</f>
-        <v>9.4710028571428587E-2</v>
+        <v>0.12047899999999999</v>
       </c>
     </row>
     <row r="121" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B121" s="1">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C121" s="1">
-        <v>142.68</v>
+        <v>144.31</v>
       </c>
       <c r="D121" s="1">
-        <v>88.59</v>
-      </c>
-      <c r="E121" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.4599999999999996E-2</v>
+        <v>105.44</v>
+      </c>
+      <c r="E121" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.8799999999999998E-2</v>
       </c>
       <c r="F121" s="1">
         <f>+((C121*$J$6)/$K$6)/1000</f>
-        <v>0.15205611428571428</v>
+        <v>0.15379322857142855</v>
       </c>
       <c r="G121" s="1">
         <f>+((D121*$J$6)/$K$6)/1000</f>
-        <v>9.4411628571428569E-2</v>
+        <v>0.11236891428571429</v>
       </c>
     </row>
     <row r="122" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B122" s="1">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C122" s="1">
-        <v>131.26</v>
+        <v>118.22</v>
       </c>
       <c r="D122" s="1">
-        <v>88.59</v>
-      </c>
-      <c r="E122" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>3.6400000000000002E-2</v>
+        <v>100.01</v>
+      </c>
+      <c r="E122" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.8799999999999998E-2</v>
       </c>
       <c r="F122" s="1">
         <f>+((C122*$J$6)/$K$6)/1000</f>
-        <v>0.13988565714285714</v>
+        <v>0.12598874285714284</v>
       </c>
       <c r="G122" s="1">
         <f>+((D122*$J$6)/$K$6)/1000</f>
-        <v>9.4411628571428569E-2</v>
+        <v>0.10658208571428571</v>
       </c>
     </row>
     <row r="123" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B123" s="1">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C123" s="1">
-        <v>118.49</v>
+        <v>145.66</v>
       </c>
       <c r="D123" s="1">
-        <v>88.32</v>
-      </c>
-      <c r="E123" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.6000000000000001E-2</v>
+        <v>91.58</v>
+      </c>
+      <c r="E123" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.8799999999999998E-2</v>
       </c>
       <c r="F123" s="1">
         <f>+((C123*$J$6)/$K$6)/1000</f>
-        <v>0.12627648571428571</v>
+        <v>0.15523194285714287</v>
       </c>
       <c r="G123" s="1">
         <f>+((D123*$J$6)/$K$6)/1000</f>
-        <v>9.4123885714285691E-2</v>
+        <v>9.7598114285714271E-2</v>
       </c>
     </row>
     <row r="124" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B124" s="1">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="C124" s="1">
-        <v>131.26</v>
+        <v>125.83</v>
       </c>
       <c r="D124" s="1">
-        <v>88.32</v>
-      </c>
-      <c r="E124" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>3.78E-2</v>
+        <v>82.34</v>
+      </c>
+      <c r="E124" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>5.8799999999999998E-2</v>
       </c>
       <c r="F124" s="1">
         <f>+((C124*$J$6)/$K$6)/1000</f>
-        <v>0.13988565714285714</v>
+        <v>0.13409882857142855</v>
       </c>
       <c r="G124" s="1">
         <f>+((D124*$J$6)/$K$6)/1000</f>
-        <v>9.4123885714285691E-2</v>
+        <v>8.7750914285714271E-2</v>
       </c>
     </row>
     <row r="125" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B125" s="1">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C125" s="1">
-        <v>135.88</v>
+        <v>129.63</v>
       </c>
       <c r="D125" s="1">
-        <v>87.78</v>
-      </c>
-      <c r="E125" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.2999999999999987E-2</v>
+        <v>112.24</v>
+      </c>
+      <c r="E125" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.0199999999999997E-2</v>
       </c>
       <c r="F125" s="1">
         <f>+((C125*$J$6)/$K$6)/1000</f>
-        <v>0.14480925714285711</v>
+        <v>0.13814854285714284</v>
       </c>
       <c r="G125" s="1">
         <f>+((D125*$J$6)/$K$6)/1000</f>
-        <v>9.3548400000000004E-2</v>
+        <v>0.11961577142857142</v>
       </c>
     </row>
     <row r="126" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B126" s="1">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C126" s="1">
-        <v>120.12</v>
+        <v>140.77000000000001</v>
       </c>
       <c r="D126" s="1">
-        <v>87.24</v>
-      </c>
-      <c r="E126" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.74E-2</v>
+        <v>107.35</v>
+      </c>
+      <c r="E126" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.0199999999999997E-2</v>
       </c>
       <c r="F126" s="1">
         <f>+((C126*$J$6)/$K$6)/1000</f>
-        <v>0.12801360000000001</v>
+        <v>0.15002059999999998</v>
       </c>
       <c r="G126" s="1">
         <f>+((D126*$J$6)/$K$6)/1000</f>
-        <v>9.2972914285714275E-2</v>
+        <v>0.11440442857142856</v>
       </c>
     </row>
     <row r="127" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B127" s="1">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="C127" s="1">
-        <v>130.16999999999999</v>
+        <v>119.3</v>
       </c>
       <c r="D127" s="1">
-        <v>87.24</v>
-      </c>
-      <c r="E127" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>3.9199999999999999E-2</v>
+        <v>98.38</v>
+      </c>
+      <c r="E127" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.0199999999999997E-2</v>
       </c>
       <c r="F127" s="1">
         <f>+((C127*$J$6)/$K$6)/1000</f>
-        <v>0.13872402857142857</v>
+        <v>0.12713971428571427</v>
       </c>
       <c r="G127" s="1">
         <f>+((D127*$J$6)/$K$6)/1000</f>
-        <v>9.2972914285714275E-2</v>
+        <v>0.10484497142857141</v>
       </c>
     </row>
     <row r="128" spans="2:7" x14ac:dyDescent="0.25">
@@ -3390,64 +3406,64 @@
         <v>43</v>
       </c>
       <c r="C128" s="1">
-        <v>121.48</v>
+        <v>146.75</v>
       </c>
       <c r="D128" s="1">
-        <v>86.96</v>
-      </c>
-      <c r="E128" s="7">
+        <v>96.75</v>
+      </c>
+      <c r="E128" s="6">
         <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
         <v>6.0199999999999997E-2</v>
       </c>
       <c r="F128" s="1">
         <f>+((C128*$J$6)/$K$6)/1000</f>
-        <v>0.12946297142857141</v>
+        <v>0.15639357142857141</v>
       </c>
       <c r="G128" s="1">
         <f>+((D128*$J$6)/$K$6)/1000</f>
-        <v>9.2674514285714285E-2</v>
+        <v>0.10310785714285713</v>
       </c>
     </row>
     <row r="129" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B129" s="1">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C129" s="1">
-        <v>136.69999999999999</v>
+        <v>121.48</v>
       </c>
       <c r="D129" s="1">
-        <v>86.69</v>
-      </c>
-      <c r="E129" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.1599999999999995E-2</v>
+        <v>86.96</v>
+      </c>
+      <c r="E129" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.0199999999999997E-2</v>
       </c>
       <c r="F129" s="1">
         <f>+((C129*$J$6)/$K$6)/1000</f>
-        <v>0.14568314285714282</v>
+        <v>0.12946297142857141</v>
       </c>
       <c r="G129" s="1">
         <f>+((D129*$J$6)/$K$6)/1000</f>
-        <v>9.2386771428571421E-2</v>
+        <v>9.2674514285714285E-2</v>
       </c>
     </row>
     <row r="130" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B130" s="1">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C130" s="1">
-        <v>130.16999999999999</v>
+        <v>136.97</v>
       </c>
       <c r="D130" s="1">
         <v>85.88</v>
       </c>
-      <c r="E130" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.7199999999999982E-2</v>
+      <c r="E130" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.0199999999999997E-2</v>
       </c>
       <c r="F130" s="1">
         <f>+((C130*$J$6)/$K$6)/1000</f>
-        <v>0.13872402857142857</v>
+        <v>0.14597088571428571</v>
       </c>
       <c r="G130" s="1">
         <f>+((D130*$J$6)/$K$6)/1000</f>
@@ -3459,160 +3475,160 @@
         <v>43</v>
       </c>
       <c r="C131" s="1">
-        <v>136.97</v>
+        <v>128.82</v>
       </c>
       <c r="D131" s="1">
-        <v>85.88</v>
-      </c>
-      <c r="E131" s="7">
+        <v>82.07</v>
+      </c>
+      <c r="E131" s="6">
         <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
         <v>6.0199999999999997E-2</v>
       </c>
       <c r="F131" s="1">
         <f>+((C131*$J$6)/$K$6)/1000</f>
-        <v>0.14597088571428571</v>
+        <v>0.13728531428571428</v>
       </c>
       <c r="G131" s="1">
         <f>+((D131*$J$6)/$K$6)/1000</f>
-        <v>9.1523542857142842E-2</v>
+        <v>8.7463171428571421E-2</v>
       </c>
     </row>
     <row r="132" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B132" s="1">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="C132" s="1">
-        <v>129.09</v>
+        <v>133.97999999999999</v>
       </c>
       <c r="D132" s="1">
-        <v>85.06</v>
-      </c>
-      <c r="E132" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.0599999999999997E-2</v>
+        <v>110.88</v>
+      </c>
+      <c r="E132" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.1599999999999995E-2</v>
       </c>
       <c r="F132" s="1">
         <f>+((C132*$J$6)/$K$6)/1000</f>
-        <v>0.13757305714285711</v>
+        <v>0.14278439999999998</v>
       </c>
       <c r="G132" s="1">
         <f>+((D132*$J$6)/$K$6)/1000</f>
-        <v>9.0649657142857137E-2</v>
+        <v>0.11816639999999999</v>
       </c>
     </row>
     <row r="133" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B133" s="1">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C133" s="1">
-        <v>130.44999999999999</v>
+        <v>122.56</v>
       </c>
       <c r="D133" s="1">
-        <v>84.79</v>
-      </c>
-      <c r="E133" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.5799999999999997E-2</v>
+        <v>103.81</v>
+      </c>
+      <c r="E133" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.1599999999999995E-2</v>
       </c>
       <c r="F133" s="1">
         <f>+((C133*$J$6)/$K$6)/1000</f>
-        <v>0.13902242857142855</v>
+        <v>0.13061394285714284</v>
       </c>
       <c r="G133" s="1">
         <f>+((D133*$J$6)/$K$6)/1000</f>
-        <v>9.0361914285714273E-2</v>
+        <v>0.1106318</v>
       </c>
     </row>
     <row r="134" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B134" s="1">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C134" s="1">
-        <v>139.41</v>
+        <v>146.47999999999999</v>
       </c>
       <c r="D134" s="1">
-        <v>83.7</v>
-      </c>
-      <c r="E134" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.6000000000000001E-2</v>
+        <v>97.83</v>
+      </c>
+      <c r="E134" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.1599999999999995E-2</v>
       </c>
       <c r="F134" s="1">
         <f>+((C134*$J$6)/$K$6)/1000</f>
-        <v>0.14857122857142854</v>
+        <v>0.15610582857142855</v>
       </c>
       <c r="G134" s="1">
         <f>+((D134*$J$6)/$K$6)/1000</f>
-        <v>8.9200285714285718E-2</v>
+        <v>0.10425882857142857</v>
       </c>
     </row>
     <row r="135" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B135" s="1">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C135" s="1">
-        <v>138.33000000000001</v>
+        <v>119.58</v>
       </c>
       <c r="D135" s="1">
-        <v>83.43</v>
-      </c>
-      <c r="E135" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.74E-2</v>
+        <v>90.77</v>
+      </c>
+      <c r="E135" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.1599999999999995E-2</v>
       </c>
       <c r="F135" s="1">
         <f>+((C135*$J$6)/$K$6)/1000</f>
-        <v>0.14742025714285714</v>
+        <v>0.12743811428571428</v>
       </c>
       <c r="G135" s="1">
         <f>+((D135*$J$6)/$K$6)/1000</f>
-        <v>8.8912542857142854E-2</v>
+        <v>9.6734885714285693E-2</v>
       </c>
     </row>
     <row r="136" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B136" s="1">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C136" s="1">
-        <v>103.17</v>
+        <v>136.69999999999999</v>
       </c>
       <c r="D136" s="1">
-        <v>83.16</v>
-      </c>
-      <c r="E136" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.4399999999999985E-2</v>
+        <v>86.69</v>
+      </c>
+      <c r="E136" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.1599999999999995E-2</v>
       </c>
       <c r="F136" s="1">
         <f>+((C136*$J$6)/$K$6)/1000</f>
-        <v>0.10994974285714285</v>
+        <v>0.14568314285714282</v>
       </c>
       <c r="G136" s="1">
         <f>+((D136*$J$6)/$K$6)/1000</f>
-        <v>8.8624799999999976E-2</v>
+        <v>9.2386771428571421E-2</v>
       </c>
     </row>
     <row r="137" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B137" s="1">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C137" s="1">
-        <v>132.88999999999999</v>
+        <v>130.16999999999999</v>
       </c>
       <c r="D137" s="1">
-        <v>82.89</v>
-      </c>
-      <c r="E137" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.2000000000000003E-2</v>
+        <v>82.62</v>
+      </c>
+      <c r="E137" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.1599999999999995E-2</v>
       </c>
       <c r="F137" s="1">
         <f>+((C137*$J$6)/$K$6)/1000</f>
-        <v>0.14162277142857138</v>
+        <v>0.13872402857142857</v>
       </c>
       <c r="G137" s="1">
         <f>+((D137*$J$6)/$K$6)/1000</f>
-        <v>8.8337057142857139E-2</v>
+        <v>8.8049314285714289E-2</v>
       </c>
     </row>
     <row r="138" spans="2:7" x14ac:dyDescent="0.25">
@@ -3620,336 +3636,336 @@
         <v>45</v>
       </c>
       <c r="C138" s="1">
-        <v>128.27000000000001</v>
+        <v>125.55</v>
       </c>
       <c r="D138" s="1">
-        <v>82.62</v>
-      </c>
-      <c r="E138" s="7">
+        <v>107.35</v>
+      </c>
+      <c r="E138" s="6">
         <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
         <v>6.2999999999999987E-2</v>
       </c>
       <c r="F138" s="1">
         <f>+((C138*$J$6)/$K$6)/1000</f>
-        <v>0.13669917142857144</v>
+        <v>0.13380042857142857</v>
       </c>
       <c r="G138" s="1">
         <f>+((D138*$J$6)/$K$6)/1000</f>
-        <v>8.8049314285714289E-2</v>
+        <v>0.11440442857142856</v>
       </c>
     </row>
     <row r="139" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B139" s="1">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C139" s="1">
-        <v>130.16999999999999</v>
+        <v>138.06</v>
       </c>
       <c r="D139" s="1">
-        <v>82.62</v>
-      </c>
-      <c r="E139" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.1599999999999995E-2</v>
+        <v>106.06</v>
+      </c>
+      <c r="E139" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.2999999999999987E-2</v>
       </c>
       <c r="F139" s="1">
         <f>+((C139*$J$6)/$K$6)/1000</f>
-        <v>0.13872402857142857</v>
+        <v>0.14713251428571428</v>
       </c>
       <c r="G139" s="1">
         <f>+((D139*$J$6)/$K$6)/1000</f>
-        <v>8.8049314285714289E-2</v>
+        <v>0.11302965714285713</v>
       </c>
     </row>
     <row r="140" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B140" s="1">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C140" s="1">
-        <v>123.38</v>
+        <v>144.85</v>
       </c>
       <c r="D140" s="1">
-        <v>82.62</v>
-      </c>
-      <c r="E140" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.4599999999999996E-2</v>
+        <v>95.39</v>
+      </c>
+      <c r="E140" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.2999999999999987E-2</v>
       </c>
       <c r="F140" s="1">
         <f>+((C140*$J$6)/$K$6)/1000</f>
-        <v>0.13148782857142857</v>
+        <v>0.15436871428571428</v>
       </c>
       <c r="G140" s="1">
         <f>+((D140*$J$6)/$K$6)/1000</f>
-        <v>8.8049314285714289E-2</v>
+        <v>0.10165848571428571</v>
       </c>
     </row>
     <row r="141" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B141" s="1">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C141" s="1">
-        <v>123.38</v>
+        <v>120.66</v>
       </c>
       <c r="D141" s="1">
-        <v>82.62</v>
-      </c>
-      <c r="E141" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.3199999999999997E-2</v>
+        <v>92.67</v>
+      </c>
+      <c r="E141" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.2999999999999987E-2</v>
       </c>
       <c r="F141" s="1">
         <f>+((C141*$J$6)/$K$6)/1000</f>
-        <v>0.13148782857142857</v>
+        <v>0.12858908571428568</v>
       </c>
       <c r="G141" s="1">
         <f>+((D141*$J$6)/$K$6)/1000</f>
-        <v>8.8049314285714289E-2</v>
+        <v>9.8759742857142854E-2</v>
       </c>
     </row>
     <row r="142" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B142" s="1">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C142" s="1">
-        <v>125.83</v>
+        <v>135.88</v>
       </c>
       <c r="D142" s="1">
-        <v>82.34</v>
-      </c>
-      <c r="E142" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.8799999999999998E-2</v>
+        <v>87.78</v>
+      </c>
+      <c r="E142" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.2999999999999987E-2</v>
       </c>
       <c r="F142" s="1">
         <f>+((C142*$J$6)/$K$6)/1000</f>
-        <v>0.13409882857142855</v>
+        <v>0.14480925714285711</v>
       </c>
       <c r="G142" s="1">
         <f>+((D142*$J$6)/$K$6)/1000</f>
-        <v>8.7750914285714271E-2</v>
+        <v>9.3548400000000004E-2</v>
       </c>
     </row>
     <row r="143" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B143" s="1">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C143" s="1">
-        <v>125.28</v>
+        <v>128.27000000000001</v>
       </c>
       <c r="D143" s="1">
-        <v>82.34</v>
-      </c>
-      <c r="E143" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.74E-2</v>
+        <v>82.62</v>
+      </c>
+      <c r="E143" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.2999999999999987E-2</v>
       </c>
       <c r="F143" s="1">
         <f>+((C143*$J$6)/$K$6)/1000</f>
-        <v>0.13351268571428571</v>
+        <v>0.13669917142857144</v>
       </c>
       <c r="G143" s="1">
         <f>+((D143*$J$6)/$K$6)/1000</f>
-        <v>8.7750914285714271E-2</v>
+        <v>8.8049314285714289E-2</v>
       </c>
     </row>
     <row r="144" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B144" s="1">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C144" s="1">
-        <v>128.82</v>
+        <v>130.99</v>
       </c>
       <c r="D144" s="1">
-        <v>82.07</v>
-      </c>
-      <c r="E144" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>6.0199999999999997E-2</v>
+        <v>107.62</v>
+      </c>
+      <c r="E144" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.4399999999999985E-2</v>
       </c>
       <c r="F144" s="1">
         <f>+((C144*$J$6)/$K$6)/1000</f>
-        <v>0.13728531428571428</v>
+        <v>0.13959791428571428</v>
       </c>
       <c r="G144" s="1">
         <f>+((D144*$J$6)/$K$6)/1000</f>
-        <v>8.7463171428571421E-2</v>
+        <v>0.11469217142857141</v>
       </c>
     </row>
     <row r="145" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B145" s="1">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C145" s="1">
-        <v>138.6</v>
+        <v>142.94999999999999</v>
       </c>
       <c r="D145" s="1">
-        <v>81.8</v>
-      </c>
-      <c r="E145" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.3199999999999997E-2</v>
+        <v>96.2</v>
+      </c>
+      <c r="E145" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.4399999999999985E-2</v>
       </c>
       <c r="F145" s="1">
         <f>+((C145*$J$6)/$K$6)/1000</f>
-        <v>0.14770800000000001</v>
+        <v>0.15234385714285711</v>
       </c>
       <c r="G145" s="1">
         <f>+((D145*$J$6)/$K$6)/1000</f>
-        <v>8.717542857142857E-2</v>
+        <v>0.10252171428571429</v>
       </c>
     </row>
     <row r="146" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B146" s="1">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C146" s="1">
-        <v>140.77000000000001</v>
+        <v>120.93</v>
       </c>
       <c r="D146" s="1">
-        <v>81.8</v>
-      </c>
-      <c r="E146" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.9000000000000002E-2</v>
+        <v>94.85</v>
+      </c>
+      <c r="E146" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.4399999999999985E-2</v>
       </c>
       <c r="F146" s="1">
         <f>+((C146*$J$6)/$K$6)/1000</f>
-        <v>0.15002059999999998</v>
+        <v>0.12887682857142857</v>
       </c>
       <c r="G146" s="1">
         <f>+((D146*$J$6)/$K$6)/1000</f>
-        <v>8.717542857142857E-2</v>
+        <v>0.10108299999999999</v>
       </c>
     </row>
     <row r="147" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B147" s="1">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C147" s="1">
-        <v>132.35</v>
+        <v>137.24</v>
       </c>
       <c r="D147" s="1">
-        <v>81.8</v>
-      </c>
-      <c r="E147" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.3400000000000001E-2</v>
+        <v>90.77</v>
+      </c>
+      <c r="E147" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.4399999999999985E-2</v>
       </c>
       <c r="F147" s="1">
         <f>+((C147*$J$6)/$K$6)/1000</f>
-        <v>0.14104728571428571</v>
+        <v>0.14625862857142857</v>
       </c>
       <c r="G147" s="1">
         <f>+((D147*$J$6)/$K$6)/1000</f>
-        <v>8.717542857142857E-2</v>
+        <v>9.6734885714285693E-2</v>
       </c>
     </row>
     <row r="148" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B148" s="1">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C148" s="1">
-        <v>125.83</v>
+        <v>131.75</v>
       </c>
       <c r="D148" s="1">
-        <v>81.53</v>
-      </c>
-      <c r="E148" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.6000000000000001E-2</v>
+        <v>83.11</v>
+      </c>
+      <c r="E148" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.4399999999999985E-2</v>
       </c>
       <c r="F148" s="1">
         <f>+((C148*$J$6)/$K$6)/1000</f>
-        <v>0.13409882857142855</v>
+        <v>0.14040785714285711</v>
       </c>
       <c r="G148" s="1">
         <f>+((D148*$J$6)/$K$6)/1000</f>
-        <v>8.6887685714285706E-2</v>
+        <v>8.8571514285714276E-2</v>
       </c>
     </row>
     <row r="149" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B149" s="1">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="C149" s="1">
-        <v>133.97999999999999</v>
+        <v>131.26</v>
       </c>
       <c r="D149" s="1">
-        <v>81.260000000000005</v>
-      </c>
-      <c r="E149" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.48E-2</v>
+        <v>103.54</v>
+      </c>
+      <c r="E149" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.5799999999999997E-2</v>
       </c>
       <c r="F149" s="1">
         <f>+((C149*$J$6)/$K$6)/1000</f>
-        <v>0.14278439999999998</v>
+        <v>0.13988565714285714</v>
       </c>
       <c r="G149" s="1">
         <f>+((D149*$J$6)/$K$6)/1000</f>
-        <v>8.659994285714287E-2</v>
+        <v>0.11034405714285714</v>
       </c>
     </row>
     <row r="150" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B150" s="1">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C150" s="1">
-        <v>132.88999999999999</v>
+        <v>138.33000000000001</v>
       </c>
       <c r="D150" s="1">
-        <v>80.989999999999995</v>
-      </c>
-      <c r="E150" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.4599999999999996E-2</v>
+        <v>95.93</v>
+      </c>
+      <c r="E150" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.5799999999999997E-2</v>
       </c>
       <c r="F150" s="1">
         <f>+((C150*$J$6)/$K$6)/1000</f>
-        <v>0.14162277142857138</v>
+        <v>0.14742025714285714</v>
       </c>
       <c r="G150" s="1">
         <f>+((D150*$J$6)/$K$6)/1000</f>
-        <v>8.6312199999999992E-2</v>
+        <v>0.10223397142857142</v>
       </c>
     </row>
     <row r="151" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B151" s="1">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C151" s="1">
-        <v>128.82</v>
+        <v>123.38</v>
       </c>
       <c r="D151" s="1">
-        <v>80.989999999999995</v>
-      </c>
-      <c r="E151" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.3199999999999997E-2</v>
+        <v>94.03</v>
+      </c>
+      <c r="E151" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.5799999999999997E-2</v>
       </c>
       <c r="F151" s="1">
         <f>+((C151*$J$6)/$K$6)/1000</f>
-        <v>0.13728531428571428</v>
+        <v>0.13148782857142857</v>
       </c>
       <c r="G151" s="1">
         <f>+((D151*$J$6)/$K$6)/1000</f>
-        <v>8.6312199999999992E-2</v>
+        <v>0.10020911428571427</v>
       </c>
     </row>
     <row r="152" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B152" s="1">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C152" s="1">
         <v>130.44999999999999</v>
       </c>
       <c r="D152" s="1">
-        <v>80.709999999999994</v>
-      </c>
-      <c r="E152" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.9000000000000002E-2</v>
+        <v>84.79</v>
+      </c>
+      <c r="E152" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.5799999999999997E-2</v>
       </c>
       <c r="F152" s="1">
         <f>+((C152*$J$6)/$K$6)/1000</f>
@@ -3957,99 +3973,99 @@
       </c>
       <c r="G152" s="1">
         <f>+((D152*$J$6)/$K$6)/1000</f>
-        <v>8.6013799999999987E-2</v>
+        <v>9.0361914285714273E-2</v>
       </c>
     </row>
     <row r="153" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B153" s="1">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="C153" s="1">
-        <v>134.25</v>
+        <v>127.46</v>
       </c>
       <c r="D153" s="1">
-        <v>80.709999999999994</v>
-      </c>
-      <c r="E153" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.6199999999999998E-2</v>
+        <v>101.64</v>
+      </c>
+      <c r="E153" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.7199999999999982E-2</v>
       </c>
       <c r="F153" s="1">
         <f>+((C153*$J$6)/$K$6)/1000</f>
-        <v>0.14307214285714284</v>
+        <v>0.13583594285714284</v>
       </c>
       <c r="G153" s="1">
         <f>+((D153*$J$6)/$K$6)/1000</f>
-        <v>8.6013799999999987E-2</v>
+        <v>0.10831919999999998</v>
       </c>
     </row>
     <row r="154" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B154" s="1">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C154" s="1">
-        <v>133.71</v>
+        <v>136.15</v>
       </c>
       <c r="D154" s="1">
-        <v>80.44</v>
-      </c>
-      <c r="E154" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.1799999999999999E-2</v>
+        <v>94.57</v>
+      </c>
+      <c r="E154" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.7199999999999982E-2</v>
       </c>
       <c r="F154" s="1">
         <f>+((C154*$J$6)/$K$6)/1000</f>
-        <v>0.14249665714285714</v>
+        <v>0.14509699999999998</v>
       </c>
       <c r="G154" s="1">
         <f>+((D154*$J$6)/$K$6)/1000</f>
-        <v>8.5726057142857137E-2</v>
+        <v>0.10078459999999999</v>
       </c>
     </row>
     <row r="155" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B155" s="1">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C155" s="1">
-        <v>133.71</v>
+        <v>123.92</v>
       </c>
       <c r="D155" s="1">
-        <v>80.17</v>
-      </c>
-      <c r="E155" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>5.04E-2</v>
+        <v>92.13</v>
+      </c>
+      <c r="E155" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.7199999999999982E-2</v>
       </c>
       <c r="F155" s="1">
         <f>+((C155*$J$6)/$K$6)/1000</f>
-        <v>0.14249665714285714</v>
+        <v>0.13206331428571425</v>
       </c>
       <c r="G155" s="1">
         <f>+((D155*$J$6)/$K$6)/1000</f>
-        <v>8.5438314285714287E-2</v>
+        <v>9.818425714285714E-2</v>
       </c>
     </row>
     <row r="156" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B156" s="1">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C156" s="1">
-        <v>134.79</v>
+        <v>130.16999999999999</v>
       </c>
       <c r="D156" s="1">
-        <v>79.900000000000006</v>
-      </c>
-      <c r="E156" s="7">
-        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
-        <v>4.7599999999999996E-2</v>
+        <v>85.88</v>
+      </c>
+      <c r="E156" s="6">
+        <f>+Tabla1[[#This Row],[Diapositiva]]*(1.4)/1000</f>
+        <v>6.7199999999999982E-2</v>
       </c>
       <c r="F156" s="1">
         <f>+((C156*$J$6)/$K$6)/1000</f>
-        <v>0.14364762857142854</v>
+        <v>0.13872402857142857</v>
       </c>
       <c r="G156" s="1">
         <f>+((D156*$J$6)/$K$6)/1000</f>
-        <v>8.5150571428571423E-2</v>
+        <v>9.1523542857142842E-2</v>
       </c>
     </row>
     <row r="157" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fiduciales mismo frame del tumor
</commit_message>
<xml_diff>
--- a/puntos del tumor.xlsx
+++ b/puntos del tumor.xlsx
@@ -81,9 +81,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -192,7 +193,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -212,14 +213,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -227,10 +222,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -568,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:S157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,6 +583,7 @@
     <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" customWidth="1"/>
     <col min="10" max="10" width="11.140625" customWidth="1"/>
+    <col min="14" max="15" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
@@ -587,10 +592,10 @@
       </c>
     </row>
     <row r="4" spans="2:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="7"/>
+      <c r="K4" s="10"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -669,12 +674,12 @@
         <f t="shared" si="1"/>
         <v>0.10455722857142857</v>
       </c>
-      <c r="P7" s="9" t="s">
+      <c r="P7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
     </row>
     <row r="8" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
@@ -698,10 +703,10 @@
         <f t="shared" si="1"/>
         <v>0.10368334285714285</v>
       </c>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
@@ -738,7 +743,7 @@
       <c r="N9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O9" s="11" t="s">
+      <c r="O9" s="9" t="s">
         <v>12</v>
       </c>
       <c r="P9" s="1" t="s">
@@ -747,7 +752,7 @@
       <c r="Q9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="R9" s="10" t="s">
+      <c r="R9" s="8" t="s">
         <v>6</v>
       </c>
     </row>
@@ -786,11 +791,11 @@
         <f>+(L10*$J$6)/$K$6</f>
         <v>130.31554285714284</v>
       </c>
-      <c r="N10" s="4">
+      <c r="N10" s="12">
         <f>+M10/1000</f>
         <v>0.13031554285714284</v>
       </c>
-      <c r="O10" s="12">
+      <c r="O10" s="13">
         <f>+J10*1.14/1000</f>
         <v>2.1659999999999995E-2</v>
       </c>
@@ -844,11 +849,11 @@
         <f>+(L11*$J$6)/$K$6</f>
         <v>221.76448571428571</v>
       </c>
-      <c r="N11" s="4">
+      <c r="N11" s="12">
         <f>+M11/1000</f>
         <v>0.22176448571428573</v>
       </c>
-      <c r="O11" s="12">
+      <c r="O11" s="13">
         <f t="shared" ref="O11:O15" si="2">+J11*1.14/1000</f>
         <v>2.1659999999999995E-2</v>
       </c>
@@ -902,11 +907,11 @@
         <f t="shared" ref="M12:M15" si="5">+(L12*$J$6)/$K$6</f>
         <v>74.514742857142863</v>
       </c>
-      <c r="N12" s="4">
+      <c r="N12" s="12">
         <f t="shared" ref="N12:N15" si="6">+M12/1000</f>
         <v>7.4514742857142865E-2</v>
       </c>
-      <c r="O12" s="12">
+      <c r="O12" s="13">
         <f t="shared" si="2"/>
         <v>9.2339999999999992E-2</v>
       </c>
@@ -960,11 +965,11 @@
         <f t="shared" si="5"/>
         <v>227.02911428571426</v>
       </c>
-      <c r="N13" s="4">
+      <c r="N13" s="12">
         <f t="shared" si="6"/>
         <v>0.22702911428571426</v>
       </c>
-      <c r="O13" s="12">
+      <c r="O13" s="13">
         <f t="shared" si="2"/>
         <v>9.2339999999999992E-2</v>
       </c>
@@ -1018,11 +1023,11 @@
         <f t="shared" si="5"/>
         <v>198.10562857142855</v>
       </c>
-      <c r="N14" s="4">
+      <c r="N14" s="12">
         <f t="shared" si="6"/>
         <v>0.19810562857142855</v>
       </c>
-      <c r="O14" s="12">
+      <c r="O14" s="13">
         <f t="shared" si="2"/>
         <v>5.4719999999999998E-2</v>
       </c>
@@ -1076,11 +1081,11 @@
         <f t="shared" si="5"/>
         <v>223.01137142857141</v>
       </c>
-      <c r="N15" s="4">
+      <c r="N15" s="12">
         <f t="shared" si="6"/>
         <v>0.22301137142857141</v>
       </c>
-      <c r="O15" s="13">
+      <c r="O15" s="14">
         <f t="shared" si="2"/>
         <v>5.4719999999999998E-2</v>
       </c>
@@ -1152,7 +1157,7 @@
         <f t="shared" si="1"/>
         <v>0.10803145714285714</v>
       </c>
-      <c r="J17" s="8" t="s">
+      <c r="J17" s="7" t="s">
         <v>7</v>
       </c>
       <c r="K17" s="1"/>

</xml_diff>